<commit_message>
Beginning the process of adding in relative temperature
</commit_message>
<xml_diff>
--- a/Excel & CSV Sheets/New Data Files/Day Holder 2017.xlsx
+++ b/Excel & CSV Sheets/New Data Files/Day Holder 2017.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Days" sheetId="1" state="visible" r:id="rId2"/>
@@ -146,12 +146,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -163,17 +163,17 @@
   </sheetPr>
   <dimension ref="A1:D366"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A322" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F359" activeCellId="0" sqref="F359"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I17" activeCellId="0" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2834008097166"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.246963562753"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.2105263157895"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.3400809716599"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -197,12 +197,6 @@
       <c r="B2" s="4" t="n">
         <v>42736</v>
       </c>
-      <c r="C2" s="0" t="n">
-        <v>44.4083333333333</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>46.3392483557</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="n">
@@ -211,12 +205,6 @@
       <c r="B3" s="4" t="n">
         <v>42737</v>
       </c>
-      <c r="C3" s="0" t="n">
-        <v>48.6414583333333</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>46.3392483557</v>
-      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="n">
@@ -225,12 +213,6 @@
       <c r="B4" s="4" t="n">
         <v>42738</v>
       </c>
-      <c r="C4" s="0" t="n">
-        <v>52.1384722222222</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>46.3392483557</v>
-      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="n">
@@ -239,12 +221,6 @@
       <c r="B5" s="4" t="n">
         <v>42739</v>
       </c>
-      <c r="C5" s="0" t="n">
-        <v>50.5988541666667</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>46.3392483557</v>
-      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="n">
@@ -253,12 +229,6 @@
       <c r="B6" s="4" t="n">
         <v>42740</v>
       </c>
-      <c r="C6" s="0" t="n">
-        <v>47.2399166666667</v>
-      </c>
-      <c r="D6" s="0" t="n">
-        <v>46.3392483557</v>
-      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="n">
@@ -267,12 +237,6 @@
       <c r="B7" s="4" t="n">
         <v>42741</v>
       </c>
-      <c r="C7" s="0" t="n">
-        <v>44.4054166666667</v>
-      </c>
-      <c r="D7" s="0" t="n">
-        <v>46.3392483557</v>
-      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="n">
@@ -281,12 +245,6 @@
       <c r="B8" s="4" t="n">
         <v>42742</v>
       </c>
-      <c r="C8" s="0" t="n">
-        <v>41.15875</v>
-      </c>
-      <c r="D8" s="0" t="n">
-        <v>46.3392483557</v>
-      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="n">
@@ -295,12 +253,6 @@
       <c r="B9" s="4" t="n">
         <v>42743</v>
       </c>
-      <c r="C9" s="0" t="n">
-        <v>38.4640104166667</v>
-      </c>
-      <c r="D9" s="0" t="n">
-        <v>46.3392483557</v>
-      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="n">
@@ -309,12 +261,6 @@
       <c r="B10" s="4" t="n">
         <v>42744</v>
       </c>
-      <c r="C10" s="0" t="n">
-        <v>37.6151388888889</v>
-      </c>
-      <c r="D10" s="0" t="n">
-        <v>46.3392483557</v>
-      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="n">
@@ -323,12 +269,6 @@
       <c r="B11" s="4" t="n">
         <v>42745</v>
       </c>
-      <c r="C11" s="0" t="n">
-        <v>38.1452083333333</v>
-      </c>
-      <c r="D11" s="0" t="n">
-        <v>46.3392483557</v>
-      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="n">
@@ -337,12 +277,6 @@
       <c r="B12" s="4" t="n">
         <v>42746</v>
       </c>
-      <c r="C12" s="0" t="n">
-        <v>39.6736742424242</v>
-      </c>
-      <c r="D12" s="0" t="n">
-        <v>46.3392483557</v>
-      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="n">
@@ -351,12 +285,6 @@
       <c r="B13" s="4" t="n">
         <v>42747</v>
       </c>
-      <c r="C13" s="0" t="n">
-        <v>41.5331944444444</v>
-      </c>
-      <c r="D13" s="0" t="n">
-        <v>46.3392483557</v>
-      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="n">
@@ -365,12 +293,6 @@
       <c r="B14" s="4" t="n">
         <v>42748</v>
       </c>
-      <c r="C14" s="0" t="n">
-        <v>43.0522756410256</v>
-      </c>
-      <c r="D14" s="0" t="n">
-        <v>46.3392483557</v>
-      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="n">
@@ -379,12 +301,6 @@
       <c r="B15" s="4" t="n">
         <v>42749</v>
       </c>
-      <c r="C15" s="0" t="n">
-        <v>44.4248511904762</v>
-      </c>
-      <c r="D15" s="0" t="n">
-        <v>46.3392483557</v>
-      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="n">
@@ -393,12 +309,6 @@
       <c r="B16" s="4" t="n">
         <v>42750</v>
       </c>
-      <c r="C16" s="0" t="n">
-        <v>45.5998611111111</v>
-      </c>
-      <c r="D16" s="0" t="n">
-        <v>46.3392483557</v>
-      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="n">
@@ -407,12 +317,6 @@
       <c r="B17" s="4" t="n">
         <v>42751</v>
       </c>
-      <c r="C17" s="0" t="n">
-        <v>46.3338802083333</v>
-      </c>
-      <c r="D17" s="0" t="n">
-        <v>46.3392483557</v>
-      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="n">
@@ -421,12 +325,6 @@
       <c r="B18" s="4" t="n">
         <v>42752</v>
       </c>
-      <c r="C18" s="0" t="n">
-        <v>47.2453431372549</v>
-      </c>
-      <c r="D18" s="0" t="n">
-        <v>46.3392483557</v>
-      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="n">
@@ -435,12 +333,6 @@
       <c r="B19" s="4" t="n">
         <v>42753</v>
       </c>
-      <c r="C19" s="0" t="n">
-        <v>47.9669907407407</v>
-      </c>
-      <c r="D19" s="0" t="n">
-        <v>46.3392483557</v>
-      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="n">
@@ -449,12 +341,6 @@
       <c r="B20" s="4" t="n">
         <v>42754</v>
       </c>
-      <c r="C20" s="0" t="n">
-        <v>48.2270394736842</v>
-      </c>
-      <c r="D20" s="0" t="n">
-        <v>46.3392483557</v>
-      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="n">
@@ -463,12 +349,6 @@
       <c r="B21" s="4" t="n">
         <v>42755</v>
       </c>
-      <c r="C21" s="0" t="n">
-        <v>48.8291458333333</v>
-      </c>
-      <c r="D21" s="0" t="n">
-        <v>46.3392483557</v>
-      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="n">
@@ -477,12 +357,6 @@
       <c r="B22" s="4" t="n">
         <v>42756</v>
       </c>
-      <c r="C22" s="0" t="n">
-        <v>49.2756944444444</v>
-      </c>
-      <c r="D22" s="0" t="n">
-        <v>46.3392483557</v>
-      </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="n">
@@ -491,12 +365,6 @@
       <c r="B23" s="4" t="n">
         <v>42757</v>
       </c>
-      <c r="C23" s="0" t="n">
-        <v>49.6811553030303</v>
-      </c>
-      <c r="D23" s="0" t="n">
-        <v>46.3392483557</v>
-      </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="n">
@@ -505,12 +373,6 @@
       <c r="B24" s="4" t="n">
         <v>42758</v>
       </c>
-      <c r="C24" s="0" t="n">
-        <v>49.725652173913</v>
-      </c>
-      <c r="D24" s="0" t="n">
-        <v>46.3392483557</v>
-      </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="n">
@@ -519,12 +381,6 @@
       <c r="B25" s="4" t="n">
         <v>42759</v>
       </c>
-      <c r="C25" s="0" t="n">
-        <v>49.5681770833333</v>
-      </c>
-      <c r="D25" s="0" t="n">
-        <v>46.3392483557</v>
-      </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="n">
@@ -533,12 +389,6 @@
       <c r="B26" s="4" t="n">
         <v>42760</v>
       </c>
-      <c r="C26" s="0" t="n">
-        <v>49.5954666666667</v>
-      </c>
-      <c r="D26" s="0" t="n">
-        <v>46.3392483557</v>
-      </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="n">
@@ -547,12 +397,6 @@
       <c r="B27" s="4" t="n">
         <v>42761</v>
       </c>
-      <c r="C27" s="0" t="n">
-        <v>49.6141826923077</v>
-      </c>
-      <c r="D27" s="0" t="n">
-        <v>46.3392483557</v>
-      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="n">
@@ -561,12 +405,6 @@
       <c r="B28" s="4" t="n">
         <v>42762</v>
       </c>
-      <c r="C28" s="0" t="n">
-        <v>49.1829320987654</v>
-      </c>
-      <c r="D28" s="0" t="n">
-        <v>46.3392483557</v>
-      </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="n">
@@ -575,12 +413,6 @@
       <c r="B29" s="4" t="n">
         <v>42763</v>
       </c>
-      <c r="C29" s="0" t="n">
-        <v>48.8453273809524</v>
-      </c>
-      <c r="D29" s="0" t="n">
-        <v>46.3392483557</v>
-      </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="n">
@@ -589,12 +421,6 @@
       <c r="B30" s="4" t="n">
         <v>42764</v>
       </c>
-      <c r="C30" s="0" t="n">
-        <v>48.564367816092</v>
-      </c>
-      <c r="D30" s="0" t="n">
-        <v>46.3392483557</v>
-      </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="n">
@@ -603,12 +429,6 @@
       <c r="B31" s="4" t="n">
         <v>42765</v>
       </c>
-      <c r="C31" s="0" t="n">
-        <v>48.3218611111111</v>
-      </c>
-      <c r="D31" s="0" t="n">
-        <v>46.3392483557</v>
-      </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="n">
@@ -617,12 +437,6 @@
       <c r="B32" s="4" t="n">
         <v>42766</v>
       </c>
-      <c r="C32" s="0" t="n">
-        <v>48.4400672043011</v>
-      </c>
-      <c r="D32" s="0" t="n">
-        <v>46.3392483557</v>
-      </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="n">
@@ -631,12 +445,6 @@
       <c r="B33" s="4" t="n">
         <v>42767</v>
       </c>
-      <c r="C33" s="0" t="n">
-        <v>48.655</v>
-      </c>
-      <c r="D33" s="0" t="n">
-        <v>48.6932561298</v>
-      </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="n">
@@ -645,12 +453,6 @@
       <c r="B34" s="4" t="n">
         <v>42768</v>
       </c>
-      <c r="C34" s="0" t="n">
-        <v>48.6799494949495</v>
-      </c>
-      <c r="D34" s="0" t="n">
-        <v>48.6932561298</v>
-      </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="n">
@@ -659,12 +461,6 @@
       <c r="B35" s="4" t="n">
         <v>42769</v>
       </c>
-      <c r="C35" s="0" t="n">
-        <v>48.4758946078431</v>
-      </c>
-      <c r="D35" s="0" t="n">
-        <v>48.6932561298</v>
-      </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="n">
@@ -673,12 +469,6 @@
       <c r="B36" s="4" t="n">
         <v>42770</v>
       </c>
-      <c r="C36" s="0" t="n">
-        <v>48.0948571428571</v>
-      </c>
-      <c r="D36" s="0" t="n">
-        <v>48.6932561298</v>
-      </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="n">
@@ -687,12 +477,6 @@
       <c r="B37" s="4" t="n">
         <v>42771</v>
       </c>
-      <c r="C37" s="0" t="n">
-        <v>47.9727777777778</v>
-      </c>
-      <c r="D37" s="0" t="n">
-        <v>48.6932561298</v>
-      </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="n">
@@ -701,12 +485,6 @@
       <c r="B38" s="4" t="n">
         <v>42772</v>
       </c>
-      <c r="C38" s="0" t="n">
-        <v>47.8606869369369</v>
-      </c>
-      <c r="D38" s="0" t="n">
-        <v>48.6932561298</v>
-      </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="3" t="n">
@@ -715,12 +493,6 @@
       <c r="B39" s="4" t="n">
         <v>42773</v>
       </c>
-      <c r="C39" s="0" t="n">
-        <v>48.0723574561403</v>
-      </c>
-      <c r="D39" s="0" t="n">
-        <v>48.6932561298</v>
-      </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="3" t="n">
@@ -729,12 +501,6 @@
       <c r="B40" s="4" t="n">
         <v>42774</v>
       </c>
-      <c r="C40" s="0" t="n">
-        <v>48.3569444444444</v>
-      </c>
-      <c r="D40" s="0" t="n">
-        <v>48.6932561298</v>
-      </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="3" t="n">
@@ -743,12 +509,6 @@
       <c r="B41" s="4" t="n">
         <v>42775</v>
       </c>
-      <c r="C41" s="0" t="n">
-        <v>48.1792916666667</v>
-      </c>
-      <c r="D41" s="0" t="n">
-        <v>48.6932561298</v>
-      </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="3" t="n">
@@ -757,12 +517,6 @@
       <c r="B42" s="4" t="n">
         <v>42776</v>
       </c>
-      <c r="C42" s="0" t="n">
-        <v>47.9805386178862</v>
-      </c>
-      <c r="D42" s="0" t="n">
-        <v>48.6932561298</v>
-      </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="3" t="n">
@@ -771,12 +525,6 @@
       <c r="B43" s="4" t="n">
         <v>42777</v>
       </c>
-      <c r="C43" s="0" t="n">
-        <v>48.1831944444444</v>
-      </c>
-      <c r="D43" s="0" t="n">
-        <v>48.6932561298</v>
-      </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="3" t="n">
@@ -785,12 +533,6 @@
       <c r="B44" s="4" t="n">
         <v>42778</v>
       </c>
-      <c r="C44" s="0" t="n">
-        <v>48.6135949612403</v>
-      </c>
-      <c r="D44" s="0" t="n">
-        <v>48.6932561298</v>
-      </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="3" t="n">
@@ -799,12 +541,6 @@
       <c r="B45" s="4" t="n">
         <v>42779</v>
       </c>
-      <c r="C45" s="0" t="n">
-        <v>48.6132386363636</v>
-      </c>
-      <c r="D45" s="0" t="n">
-        <v>48.6932561298</v>
-      </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="3" t="n">
@@ -813,12 +549,6 @@
       <c r="B46" s="4" t="n">
         <v>42780</v>
       </c>
-      <c r="C46" s="0" t="n">
-        <v>48.5245</v>
-      </c>
-      <c r="D46" s="0" t="n">
-        <v>48.6932561298</v>
-      </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="3" t="n">
@@ -827,12 +557,6 @@
       <c r="B47" s="4" t="n">
         <v>42781</v>
       </c>
-      <c r="C47" s="0" t="n">
-        <v>48.4924365942029</v>
-      </c>
-      <c r="D47" s="0" t="n">
-        <v>48.6932561298</v>
-      </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="3" t="n">
@@ -841,12 +565,6 @@
       <c r="B48" s="4" t="n">
         <v>42782</v>
       </c>
-      <c r="C48" s="0" t="n">
-        <v>48.3830673758865</v>
-      </c>
-      <c r="D48" s="0" t="n">
-        <v>48.6932561298</v>
-      </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="3" t="n">
@@ -855,12 +573,6 @@
       <c r="B49" s="4" t="n">
         <v>42783</v>
       </c>
-      <c r="C49" s="0" t="n">
-        <v>48.4217274305555</v>
-      </c>
-      <c r="D49" s="0" t="n">
-        <v>48.6932561298</v>
-      </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="3" t="n">
@@ -869,12 +581,6 @@
       <c r="B50" s="4" t="n">
         <v>42784</v>
       </c>
-      <c r="C50" s="0" t="n">
-        <v>48.4545833333333</v>
-      </c>
-      <c r="D50" s="0" t="n">
-        <v>48.6932561298</v>
-      </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="3" t="n">
@@ -883,12 +589,6 @@
       <c r="B51" s="4" t="n">
         <v>42785</v>
       </c>
-      <c r="C51" s="0" t="n">
-        <v>48.605925</v>
-      </c>
-      <c r="D51" s="0" t="n">
-        <v>48.6932561298</v>
-      </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="3" t="n">
@@ -897,12 +597,6 @@
       <c r="B52" s="4" t="n">
         <v>42786</v>
       </c>
-      <c r="C52" s="0" t="n">
-        <v>48.7415931372549</v>
-      </c>
-      <c r="D52" s="0" t="n">
-        <v>48.6932561298</v>
-      </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="3" t="n">
@@ -911,12 +605,6 @@
       <c r="B53" s="4" t="n">
         <v>42787</v>
       </c>
-      <c r="C53" s="0" t="n">
-        <v>48.9430448717948</v>
-      </c>
-      <c r="D53" s="0" t="n">
-        <v>48.6932561298</v>
-      </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="3" t="n">
@@ -925,12 +613,6 @@
       <c r="B54" s="4" t="n">
         <v>42788</v>
       </c>
-      <c r="C54" s="0" t="n">
-        <v>49.1531996855346</v>
-      </c>
-      <c r="D54" s="0" t="n">
-        <v>48.6932561298</v>
-      </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="3" t="n">
@@ -939,12 +621,6 @@
       <c r="B55" s="4" t="n">
         <v>42789</v>
       </c>
-      <c r="C55" s="0" t="n">
-        <v>49.3966589506173</v>
-      </c>
-      <c r="D55" s="0" t="n">
-        <v>48.6932561298</v>
-      </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="3" t="n">
@@ -953,12 +629,6 @@
       <c r="B56" s="4" t="n">
         <v>42790</v>
       </c>
-      <c r="C56" s="0" t="n">
-        <v>49.7108863636363</v>
-      </c>
-      <c r="D56" s="0" t="n">
-        <v>48.6932561298</v>
-      </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="3" t="n">
@@ -967,12 +637,6 @@
       <c r="B57" s="4" t="n">
         <v>42791</v>
       </c>
-      <c r="C57" s="0" t="n">
-        <v>49.8371130952381</v>
-      </c>
-      <c r="D57" s="0" t="n">
-        <v>48.6932561298</v>
-      </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="3" t="n">
@@ -981,12 +645,6 @@
       <c r="B58" s="4" t="n">
         <v>42792</v>
       </c>
-      <c r="C58" s="0" t="n">
-        <v>49.6913742690058</v>
-      </c>
-      <c r="D58" s="0" t="n">
-        <v>48.6932561298</v>
-      </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="3" t="n">
@@ -995,12 +653,6 @@
       <c r="B59" s="4" t="n">
         <v>42793</v>
       </c>
-      <c r="C59" s="0" t="n">
-        <v>49.6236350574713</v>
-      </c>
-      <c r="D59" s="0" t="n">
-        <v>48.6932561298</v>
-      </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="3" t="n">
@@ -1009,12 +661,6 @@
       <c r="B60" s="4" t="n">
         <v>42794</v>
       </c>
-      <c r="C60" s="0" t="n">
-        <v>49.6931002824859</v>
-      </c>
-      <c r="D60" s="0" t="n">
-        <v>48.6932561298</v>
-      </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="3" t="n">
@@ -1023,12 +669,6 @@
       <c r="B61" s="4" t="n">
         <v>42795</v>
       </c>
-      <c r="C61" s="0" t="n">
-        <v>49.9202152777778</v>
-      </c>
-      <c r="D61" s="0" t="n">
-        <v>49.960553598</v>
-      </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="3" t="n">
@@ -1037,12 +677,6 @@
       <c r="B62" s="4" t="n">
         <v>42796</v>
       </c>
-      <c r="C62" s="0" t="n">
-        <v>49.8835245901639</v>
-      </c>
-      <c r="D62" s="0" t="n">
-        <v>49.960553598</v>
-      </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="3" t="n">
@@ -1051,12 +685,6 @@
       <c r="B63" s="4" t="n">
         <v>42797</v>
       </c>
-      <c r="C63" s="0" t="n">
-        <v>49.755127688172</v>
-      </c>
-      <c r="D63" s="0" t="n">
-        <v>49.960553598</v>
-      </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="3" t="n">
@@ -1065,12 +693,6 @@
       <c r="B64" s="4" t="n">
         <v>42798</v>
       </c>
-      <c r="C64" s="0" t="n">
-        <v>49.6723809523809</v>
-      </c>
-      <c r="D64" s="0" t="n">
-        <v>49.960553598</v>
-      </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="3" t="n">
@@ -1079,12 +701,6 @@
       <c r="B65" s="4" t="n">
         <v>42799</v>
       </c>
-      <c r="C65" s="0" t="n">
-        <v>49.70771484375</v>
-      </c>
-      <c r="D65" s="0" t="n">
-        <v>49.960553598</v>
-      </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="3" t="n">
@@ -1093,12 +709,6 @@
       <c r="B66" s="4" t="n">
         <v>42800</v>
       </c>
-      <c r="C66" s="0" t="n">
-        <v>49.8723397435897</v>
-      </c>
-      <c r="D66" s="0" t="n">
-        <v>49.960553598</v>
-      </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="3" t="n">
@@ -1107,12 +717,6 @@
       <c r="B67" s="4" t="n">
         <v>42801</v>
       </c>
-      <c r="C67" s="0" t="n">
-        <v>50.0173547979798</v>
-      </c>
-      <c r="D67" s="0" t="n">
-        <v>49.960553598</v>
-      </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="3" t="n">
@@ -1121,12 +725,6 @@
       <c r="B68" s="4" t="n">
         <v>42802</v>
       </c>
-      <c r="C68" s="0" t="n">
-        <v>50.1036131840796</v>
-      </c>
-      <c r="D68" s="0" t="n">
-        <v>49.960553598</v>
-      </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="3" t="n">
@@ -1135,12 +733,6 @@
       <c r="B69" s="4" t="n">
         <v>42803</v>
       </c>
-      <c r="C69" s="0" t="n">
-        <v>50.1829718137255</v>
-      </c>
-      <c r="D69" s="0" t="n">
-        <v>49.960553598</v>
-      </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="3" t="n">
@@ -1149,12 +741,6 @@
       <c r="B70" s="4" t="n">
         <v>42804</v>
       </c>
-      <c r="C70" s="0" t="n">
-        <v>50.2760929951691</v>
-      </c>
-      <c r="D70" s="0" t="n">
-        <v>49.960553598</v>
-      </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="3" t="n">
@@ -1163,12 +749,6 @@
       <c r="B71" s="4" t="n">
         <v>42805</v>
       </c>
-      <c r="C71" s="0" t="n">
-        <v>50.1169464285714</v>
-      </c>
-      <c r="D71" s="0" t="n">
-        <v>49.960553598</v>
-      </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="3" t="n">
@@ -1177,12 +757,6 @@
       <c r="B72" s="4" t="n">
         <v>42806</v>
       </c>
-      <c r="C72" s="0" t="n">
-        <v>49.9880927230047</v>
-      </c>
-      <c r="D72" s="0" t="n">
-        <v>49.960553598</v>
-      </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="3" t="n">
@@ -1191,12 +765,6 @@
       <c r="B73" s="4" t="n">
         <v>42807</v>
       </c>
-      <c r="C73" s="0" t="n">
-        <v>49.8475520833333</v>
-      </c>
-      <c r="D73" s="0" t="n">
-        <v>49.960553598</v>
-      </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="3" t="n">
@@ -1205,12 +773,6 @@
       <c r="B74" s="4" t="n">
         <v>42808</v>
       </c>
-      <c r="C74" s="0" t="n">
-        <v>49.6702625570776</v>
-      </c>
-      <c r="D74" s="0" t="n">
-        <v>49.960553598</v>
-      </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="3" t="n">
@@ -1219,12 +781,6 @@
       <c r="B75" s="4" t="n">
         <v>42809</v>
       </c>
-      <c r="C75" s="0" t="n">
-        <v>49.4264752252252</v>
-      </c>
-      <c r="D75" s="0" t="n">
-        <v>49.960553598</v>
-      </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="3" t="n">
@@ -1233,12 +789,6 @@
       <c r="B76" s="4" t="n">
         <v>42810</v>
       </c>
-      <c r="C76" s="0" t="n">
-        <v>49.2391944444444</v>
-      </c>
-      <c r="D76" s="0" t="n">
-        <v>49.960553598</v>
-      </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="3" t="n">
@@ -1247,12 +797,6 @@
       <c r="B77" s="4" t="n">
         <v>42811</v>
       </c>
-      <c r="C77" s="0" t="n">
-        <v>49.2038322368421</v>
-      </c>
-      <c r="D77" s="0" t="n">
-        <v>49.960553598</v>
-      </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="3" t="n">
@@ -1261,12 +805,6 @@
       <c r="B78" s="4" t="n">
         <v>42812</v>
       </c>
-      <c r="C78" s="0" t="n">
-        <v>49.3741504329004</v>
-      </c>
-      <c r="D78" s="0" t="n">
-        <v>49.960553598</v>
-      </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="3" t="n">
@@ -1275,12 +813,6 @@
       <c r="B79" s="4" t="n">
         <v>42813</v>
       </c>
-      <c r="C79" s="0" t="n">
-        <v>49.366266025641</v>
-      </c>
-      <c r="D79" s="0" t="n">
-        <v>49.960553598</v>
-      </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="3" t="n">
@@ -1289,12 +821,6 @@
       <c r="B80" s="4" t="n">
         <v>42814</v>
       </c>
-      <c r="C80" s="0" t="n">
-        <v>49.4239082278481</v>
-      </c>
-      <c r="D80" s="0" t="n">
-        <v>49.960553598</v>
-      </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="3" t="n">
@@ -1303,12 +829,6 @@
       <c r="B81" s="4" t="n">
         <v>42815</v>
       </c>
-      <c r="C81" s="0" t="n">
-        <v>49.6606354166666</v>
-      </c>
-      <c r="D81" s="0" t="n">
-        <v>49.960553598</v>
-      </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="3" t="n">
@@ -1317,12 +837,6 @@
       <c r="B82" s="4" t="n">
         <v>42816</v>
       </c>
-      <c r="C82" s="0" t="n">
-        <v>49.7486471193415</v>
-      </c>
-      <c r="D82" s="0" t="n">
-        <v>49.960553598</v>
-      </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="3" t="n">
@@ -1331,12 +845,6 @@
       <c r="B83" s="4" t="n">
         <v>42817</v>
       </c>
-      <c r="C83" s="0" t="n">
-        <v>49.7953810975609</v>
-      </c>
-      <c r="D83" s="0" t="n">
-        <v>49.960553598</v>
-      </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="3" t="n">
@@ -1345,12 +853,6 @@
       <c r="B84" s="4" t="n">
         <v>42818</v>
       </c>
-      <c r="C84" s="0" t="n">
-        <v>49.9378062248996</v>
-      </c>
-      <c r="D84" s="0" t="n">
-        <v>49.960553598</v>
-      </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="3" t="n">
@@ -1359,12 +861,6 @@
       <c r="B85" s="4" t="n">
         <v>42819</v>
       </c>
-      <c r="C85" s="0" t="n">
-        <v>50.1474454365079</v>
-      </c>
-      <c r="D85" s="0" t="n">
-        <v>49.960553598</v>
-      </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="3" t="n">
@@ -1373,12 +869,6 @@
       <c r="B86" s="4" t="n">
         <v>42820</v>
       </c>
-      <c r="C86" s="0" t="n">
-        <v>50.3175735294117</v>
-      </c>
-      <c r="D86" s="0" t="n">
-        <v>49.960553598</v>
-      </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="3" t="n">
@@ -1387,12 +877,6 @@
       <c r="B87" s="4" t="n">
         <v>42821</v>
       </c>
-      <c r="C87" s="0" t="n">
-        <v>50.4892054263565</v>
-      </c>
-      <c r="D87" s="0" t="n">
-        <v>49.960553598</v>
-      </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="3" t="n">
@@ -1401,12 +885,6 @@
       <c r="B88" s="4" t="n">
         <v>42822</v>
       </c>
-      <c r="C88" s="0" t="n">
-        <v>50.6485392720306</v>
-      </c>
-      <c r="D88" s="0" t="n">
-        <v>49.960553598</v>
-      </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="3" t="n">
@@ -1415,12 +893,6 @@
       <c r="B89" s="4" t="n">
         <v>42823</v>
       </c>
-      <c r="C89" s="0" t="n">
-        <v>50.8104876893939</v>
-      </c>
-      <c r="D89" s="0" t="n">
-        <v>49.960553598</v>
-      </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="3" t="n">
@@ -1429,12 +901,6 @@
       <c r="B90" s="4" t="n">
         <v>42824</v>
       </c>
-      <c r="C90" s="0" t="n">
-        <v>51.0319147940074</v>
-      </c>
-      <c r="D90" s="0" t="n">
-        <v>49.960553598</v>
-      </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="3" t="n">
@@ -1443,12 +909,6 @@
       <c r="B91" s="4" t="n">
         <v>42825</v>
       </c>
-      <c r="C91" s="0" t="n">
-        <v>51.1415092592592</v>
-      </c>
-      <c r="D91" s="0" t="n">
-        <v>49.960553598</v>
-      </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="3" t="n">
@@ -1457,12 +917,6 @@
       <c r="B92" s="4" t="n">
         <v>42826</v>
       </c>
-      <c r="C92" s="0" t="n">
-        <v>51.2246199633699</v>
-      </c>
-      <c r="D92" s="0" t="n">
-        <v>52.9694319284</v>
-      </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="3" t="n">
@@ -1471,12 +925,6 @@
       <c r="B93" s="4" t="n">
         <v>42827</v>
       </c>
-      <c r="C93" s="0" t="n">
-        <v>51.3323822463768</v>
-      </c>
-      <c r="D93" s="0" t="n">
-        <v>52.9694319284</v>
-      </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="3" t="n">
@@ -1485,12 +933,6 @@
       <c r="B94" s="4" t="n">
         <v>42828</v>
       </c>
-      <c r="C94" s="0" t="n">
-        <v>51.4836424731182</v>
-      </c>
-      <c r="D94" s="0" t="n">
-        <v>52.9694319284</v>
-      </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="3" t="n">
@@ -1499,12 +941,6 @@
       <c r="B95" s="4" t="n">
         <v>42829</v>
       </c>
-      <c r="C95" s="0" t="n">
-        <v>51.6786613475177</v>
-      </c>
-      <c r="D95" s="0" t="n">
-        <v>52.9694319284</v>
-      </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="3" t="n">
@@ -1513,12 +949,6 @@
       <c r="B96" s="4" t="n">
         <v>42830</v>
       </c>
-      <c r="C96" s="0" t="n">
-        <v>51.7861666666666</v>
-      </c>
-      <c r="D96" s="0" t="n">
-        <v>52.9694319284</v>
-      </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="3" t="n">
@@ -1527,12 +957,6 @@
       <c r="B97" s="4" t="n">
         <v>42831</v>
       </c>
-      <c r="C97" s="0" t="n">
-        <v>51.7776909722222</v>
-      </c>
-      <c r="D97" s="0" t="n">
-        <v>52.9694319284</v>
-      </c>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="3" t="n">
@@ -1541,12 +965,6 @@
       <c r="B98" s="4" t="n">
         <v>42832</v>
       </c>
-      <c r="C98" s="0" t="n">
-        <v>51.7749226804123</v>
-      </c>
-      <c r="D98" s="0" t="n">
-        <v>52.9694319284</v>
-      </c>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="3" t="n">
@@ -1555,12 +973,6 @@
       <c r="B99" s="4" t="n">
         <v>42833</v>
       </c>
-      <c r="C99" s="0" t="n">
-        <v>51.7926573129251</v>
-      </c>
-      <c r="D99" s="0" t="n">
-        <v>52.9694319284</v>
-      </c>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="3" t="n">
@@ -1569,12 +981,6 @@
       <c r="B100" s="4" t="n">
         <v>42834</v>
       </c>
-      <c r="C100" s="0" t="n">
-        <v>51.8712752525252</v>
-      </c>
-      <c r="D100" s="0" t="n">
-        <v>52.9694319284</v>
-      </c>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="3" t="n">
@@ -1583,12 +989,6 @@
       <c r="B101" s="4" t="n">
         <v>42835</v>
       </c>
-      <c r="C101" s="0" t="n">
-        <v>52.0370833333333</v>
-      </c>
-      <c r="D101" s="0" t="n">
-        <v>52.9694319284</v>
-      </c>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="3" t="n">
@@ -1597,12 +997,6 @@
       <c r="B102" s="4" t="n">
         <v>42836</v>
       </c>
-      <c r="C102" s="0" t="n">
-        <v>52.2096452145214</v>
-      </c>
-      <c r="D102" s="0" t="n">
-        <v>52.9694319284</v>
-      </c>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="3" t="n">
@@ -1611,12 +1005,6 @@
       <c r="B103" s="4" t="n">
         <v>42837</v>
       </c>
-      <c r="C103" s="0" t="n">
-        <v>52.3854207516339</v>
-      </c>
-      <c r="D103" s="0" t="n">
-        <v>52.9694319284</v>
-      </c>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="3" t="n">
@@ -1625,12 +1013,6 @@
       <c r="B104" s="4" t="n">
         <v>42838</v>
       </c>
-      <c r="C104" s="0" t="n">
-        <v>52.5530744336569</v>
-      </c>
-      <c r="D104" s="0" t="n">
-        <v>52.9694319284</v>
-      </c>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="3" t="n">
@@ -1639,12 +1021,6 @@
       <c r="B105" s="4" t="n">
         <v>42839</v>
       </c>
-      <c r="C105" s="0" t="n">
-        <v>52.7243629807692</v>
-      </c>
-      <c r="D105" s="0" t="n">
-        <v>52.9694319284</v>
-      </c>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="3" t="n">
@@ -1653,12 +1029,6 @@
       <c r="B106" s="4" t="n">
         <v>42840</v>
       </c>
-      <c r="C106" s="0" t="n">
-        <v>52.9086547619047</v>
-      </c>
-      <c r="D106" s="0" t="n">
-        <v>52.9694319284</v>
-      </c>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="3" t="n">
@@ -1667,12 +1037,6 @@
       <c r="B107" s="4" t="n">
         <v>42841</v>
       </c>
-      <c r="C107" s="0" t="n">
-        <v>53.0908726415094</v>
-      </c>
-      <c r="D107" s="0" t="n">
-        <v>52.9694319284</v>
-      </c>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="3" t="n">
@@ -1681,12 +1045,6 @@
       <c r="B108" s="4" t="n">
         <v>42842</v>
       </c>
-      <c r="C108" s="0" t="n">
-        <v>53.2500350467289</v>
-      </c>
-      <c r="D108" s="0" t="n">
-        <v>52.9694319284</v>
-      </c>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="3" t="n">
@@ -1695,12 +1053,6 @@
       <c r="B109" s="4" t="n">
         <v>42843</v>
       </c>
-      <c r="C109" s="0" t="n">
-        <v>53.3644444444444</v>
-      </c>
-      <c r="D109" s="0" t="n">
-        <v>52.9694319284</v>
-      </c>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="3" t="n">
@@ -1709,12 +1061,6 @@
       <c r="B110" s="4" t="n">
         <v>42844</v>
       </c>
-      <c r="C110" s="0" t="n">
-        <v>53.4971253822629</v>
-      </c>
-      <c r="D110" s="0" t="n">
-        <v>52.9694319284</v>
-      </c>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="3" t="n">
@@ -1723,12 +1069,6 @@
       <c r="B111" s="4" t="n">
         <v>42845</v>
       </c>
-      <c r="C111" s="0" t="n">
-        <v>53.6631553030303</v>
-      </c>
-      <c r="D111" s="0" t="n">
-        <v>52.9694319284</v>
-      </c>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="3" t="n">
@@ -1737,12 +1077,6 @@
       <c r="B112" s="4" t="n">
         <v>42846</v>
       </c>
-      <c r="C112" s="0" t="n">
-        <v>53.8316253753753</v>
-      </c>
-      <c r="D112" s="0" t="n">
-        <v>52.9694319284</v>
-      </c>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="3" t="n">
@@ -1751,12 +1085,6 @@
       <c r="B113" s="4" t="n">
         <v>42847</v>
       </c>
-      <c r="C113" s="0" t="n">
-        <v>53.9469456845238</v>
-      </c>
-      <c r="D113" s="0" t="n">
-        <v>52.9694319284</v>
-      </c>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="3" t="n">
@@ -1765,12 +1093,6 @@
       <c r="B114" s="4" t="n">
         <v>42848</v>
       </c>
-      <c r="C114" s="0" t="n">
-        <v>54.0030715339233</v>
-      </c>
-      <c r="D114" s="0" t="n">
-        <v>52.9694319284</v>
-      </c>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="3" t="n">
@@ -1779,12 +1101,6 @@
       <c r="B115" s="4" t="n">
         <v>42849</v>
       </c>
-      <c r="C115" s="0" t="n">
-        <v>54.0484722222222</v>
-      </c>
-      <c r="D115" s="0" t="n">
-        <v>52.9694319284</v>
-      </c>
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="3" t="n">
@@ -1793,12 +1109,6 @@
       <c r="B116" s="4" t="n">
         <v>42850</v>
       </c>
-      <c r="C116" s="0" t="n">
-        <v>54.140018115942</v>
-      </c>
-      <c r="D116" s="0" t="n">
-        <v>52.9694319284</v>
-      </c>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="3" t="n">
@@ -1807,12 +1117,6 @@
       <c r="B117" s="4" t="n">
         <v>42851</v>
       </c>
-      <c r="C117" s="0" t="n">
-        <v>54.2630783045977</v>
-      </c>
-      <c r="D117" s="0" t="n">
-        <v>52.9694319284</v>
-      </c>
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="3" t="n">
@@ -1821,12 +1125,6 @@
       <c r="B118" s="4" t="n">
         <v>42852</v>
       </c>
-      <c r="C118" s="0" t="n">
-        <v>54.3959366096866</v>
-      </c>
-      <c r="D118" s="0" t="n">
-        <v>52.9694319284</v>
-      </c>
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="3" t="n">
@@ -1835,12 +1133,6 @@
       <c r="B119" s="4" t="n">
         <v>42853</v>
       </c>
-      <c r="C119" s="0" t="n">
-        <v>54.5046786723164</v>
-      </c>
-      <c r="D119" s="0" t="n">
-        <v>52.9694319284</v>
-      </c>
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="3" t="n">
@@ -1849,12 +1141,6 @@
       <c r="B120" s="4" t="n">
         <v>42854</v>
       </c>
-      <c r="C120" s="0" t="n">
-        <v>54.694824929972</v>
-      </c>
-      <c r="D120" s="0" t="n">
-        <v>52.9694319284</v>
-      </c>
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="3" t="n">
@@ -1863,12 +1149,6 @@
       <c r="B121" s="4" t="n">
         <v>42855</v>
       </c>
-      <c r="C121" s="0" t="n">
-        <v>54.8484131944444</v>
-      </c>
-      <c r="D121" s="0" t="n">
-        <v>52.9694319284</v>
-      </c>
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="3" t="n">
@@ -1877,12 +1157,6 @@
       <c r="B122" s="4" t="n">
         <v>42856</v>
       </c>
-      <c r="C122" s="0" t="n">
-        <v>54.9499345730027</v>
-      </c>
-      <c r="D122" s="0" t="n">
-        <v>56.2091765322</v>
-      </c>
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="3" t="n">
@@ -1891,12 +1165,6 @@
       <c r="B123" s="4" t="n">
         <v>42857</v>
       </c>
-      <c r="C123" s="0" t="n">
-        <v>55.0256489071038</v>
-      </c>
-      <c r="D123" s="0" t="n">
-        <v>56.2091765322</v>
-      </c>
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="3" t="n">
@@ -1905,12 +1173,6 @@
       <c r="B124" s="4" t="n">
         <v>42858</v>
       </c>
-      <c r="C124" s="0" t="n">
-        <v>55.1164058265582</v>
-      </c>
-      <c r="D124" s="0" t="n">
-        <v>56.2091765322</v>
-      </c>
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="3" t="n">
@@ -1919,12 +1181,6 @@
       <c r="B125" s="4" t="n">
         <v>42859</v>
       </c>
-      <c r="C125" s="0" t="n">
-        <v>55.1871841397849</v>
-      </c>
-      <c r="D125" s="0" t="n">
-        <v>56.2091765322</v>
-      </c>
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="3" t="n">
@@ -1933,12 +1189,6 @@
       <c r="B126" s="4" t="n">
         <v>42860</v>
       </c>
-      <c r="C126" s="0" t="n">
-        <v>55.17232</v>
-      </c>
-      <c r="D126" s="0" t="n">
-        <v>56.2091765322</v>
-      </c>
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="3" t="n">
@@ -1947,12 +1197,6 @@
       <c r="B127" s="4" t="n">
         <v>42861</v>
       </c>
-      <c r="C127" s="0" t="n">
-        <v>55.1530456349206</v>
-      </c>
-      <c r="D127" s="0" t="n">
-        <v>56.2091765322</v>
-      </c>
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="3" t="n">
@@ -1961,12 +1205,6 @@
       <c r="B128" s="4" t="n">
         <v>42862</v>
       </c>
-      <c r="C128" s="0" t="n">
-        <v>55.1593602362205</v>
-      </c>
-      <c r="D128" s="0" t="n">
-        <v>56.2091765322</v>
-      </c>
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="3" t="n">
@@ -1975,12 +1213,6 @@
       <c r="B129" s="4" t="n">
         <v>42863</v>
       </c>
-      <c r="C129" s="0" t="n">
-        <v>55.2069270833333</v>
-      </c>
-      <c r="D129" s="0" t="n">
-        <v>56.2091765322</v>
-      </c>
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="3" t="n">
@@ -1989,12 +1221,6 @@
       <c r="B130" s="4" t="n">
         <v>42864</v>
       </c>
-      <c r="C130" s="0" t="n">
-        <v>55.3259496124031</v>
-      </c>
-      <c r="D130" s="0" t="n">
-        <v>56.2091765322</v>
-      </c>
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="3" t="n">
@@ -2003,12 +1229,6 @@
       <c r="B131" s="4" t="n">
         <v>42865</v>
       </c>
-      <c r="C131" s="0" t="n">
-        <v>55.4625096153846</v>
-      </c>
-      <c r="D131" s="0" t="n">
-        <v>56.2091765322</v>
-      </c>
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="3" t="n">
@@ -2017,12 +1237,6 @@
       <c r="B132" s="4" t="n">
         <v>42866</v>
       </c>
-      <c r="C132" s="0" t="n">
-        <v>55.5975667938931</v>
-      </c>
-      <c r="D132" s="0" t="n">
-        <v>56.2091765322</v>
-      </c>
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="3" t="n">
@@ -2031,12 +1245,6 @@
       <c r="B133" s="4" t="n">
         <v>42867</v>
       </c>
-      <c r="C133" s="0" t="n">
-        <v>55.7110732323232</v>
-      </c>
-      <c r="D133" s="0" t="n">
-        <v>56.2091765322</v>
-      </c>
     </row>
     <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="3" t="n">
@@ -2045,12 +1253,6 @@
       <c r="B134" s="4" t="n">
         <v>42868</v>
       </c>
-      <c r="C134" s="0" t="n">
-        <v>55.7963032581454</v>
-      </c>
-      <c r="D134" s="0" t="n">
-        <v>56.2091765322</v>
-      </c>
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="3" t="n">
@@ -2059,12 +1261,6 @@
       <c r="B135" s="4" t="n">
         <v>42869</v>
       </c>
-      <c r="C135" s="0" t="n">
-        <v>55.8803233830846</v>
-      </c>
-      <c r="D135" s="0" t="n">
-        <v>56.2091765322</v>
-      </c>
     </row>
     <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="3" t="n">
@@ -2073,12 +1269,6 @@
       <c r="B136" s="4" t="n">
         <v>42870</v>
       </c>
-      <c r="C136" s="0" t="n">
-        <v>55.9939228395062</v>
-      </c>
-      <c r="D136" s="0" t="n">
-        <v>56.2091765322</v>
-      </c>
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="3" t="n">
@@ -2087,12 +1277,6 @@
       <c r="B137" s="4" t="n">
         <v>42871</v>
       </c>
-      <c r="C137" s="0" t="n">
-        <v>56.1331433823529</v>
-      </c>
-      <c r="D137" s="0" t="n">
-        <v>56.2091765322</v>
-      </c>
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="3" t="n">
@@ -2101,12 +1285,6 @@
       <c r="B138" s="4" t="n">
         <v>42872</v>
       </c>
-      <c r="C138" s="0" t="n">
-        <v>56.2816697080292</v>
-      </c>
-      <c r="D138" s="0" t="n">
-        <v>56.2091765322</v>
-      </c>
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="3" t="n">
@@ -2115,12 +1293,6 @@
       <c r="B139" s="4" t="n">
         <v>42873</v>
       </c>
-      <c r="C139" s="0" t="n">
-        <v>56.4431461352657</v>
-      </c>
-      <c r="D139" s="0" t="n">
-        <v>56.2091765322</v>
-      </c>
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="3" t="n">
@@ -2129,12 +1301,6 @@
       <c r="B140" s="4" t="n">
         <v>42874</v>
       </c>
-      <c r="C140" s="0" t="n">
-        <v>56.5955215827338</v>
-      </c>
-      <c r="D140" s="0" t="n">
-        <v>56.2091765322</v>
-      </c>
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="3" t="n">
@@ -2143,12 +1309,6 @@
       <c r="B141" s="4" t="n">
         <v>42875</v>
       </c>
-      <c r="C141" s="0" t="n">
-        <v>56.7531279761905</v>
-      </c>
-      <c r="D141" s="0" t="n">
-        <v>56.2091765322</v>
-      </c>
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="3" t="n">
@@ -2157,12 +1317,6 @@
       <c r="B142" s="4" t="n">
         <v>42876</v>
       </c>
-      <c r="C142" s="0" t="n">
-        <v>56.8589982269504</v>
-      </c>
-      <c r="D142" s="0" t="n">
-        <v>56.2091765322</v>
-      </c>
     </row>
     <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="3" t="n">
@@ -2171,12 +1325,6 @@
       <c r="B143" s="4" t="n">
         <v>42877</v>
       </c>
-      <c r="C143" s="0" t="n">
-        <v>56.9553550469483</v>
-      </c>
-      <c r="D143" s="0" t="n">
-        <v>56.2091765322</v>
-      </c>
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="3" t="n">
@@ -2185,12 +1333,6 @@
       <c r="B144" s="4" t="n">
         <v>42878</v>
       </c>
-      <c r="C144" s="0" t="n">
-        <v>57.0290559440559</v>
-      </c>
-      <c r="D144" s="0" t="n">
-        <v>56.2091765322</v>
-      </c>
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="3" t="n">
@@ -2199,12 +1341,6 @@
       <c r="B145" s="4" t="n">
         <v>42879</v>
       </c>
-      <c r="C145" s="0" t="n">
-        <v>57.0794936342592</v>
-      </c>
-      <c r="D145" s="0" t="n">
-        <v>56.2091765322</v>
-      </c>
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="3" t="n">
@@ -2213,12 +1349,6 @@
       <c r="B146" s="4" t="n">
         <v>42880</v>
       </c>
-      <c r="C146" s="0" t="n">
-        <v>57.1069827586207</v>
-      </c>
-      <c r="D146" s="0" t="n">
-        <v>56.2091765322</v>
-      </c>
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="3" t="n">
@@ -2227,12 +1357,6 @@
       <c r="B147" s="4" t="n">
         <v>42881</v>
       </c>
-      <c r="C147" s="0" t="n">
-        <v>57.1754765981735</v>
-      </c>
-      <c r="D147" s="0" t="n">
-        <v>56.2091765322</v>
-      </c>
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="3" t="n">
@@ -2241,12 +1365,6 @@
       <c r="B148" s="4" t="n">
         <v>42882</v>
       </c>
-      <c r="C148" s="0" t="n">
-        <v>57.2894416099773</v>
-      </c>
-      <c r="D148" s="0" t="n">
-        <v>56.2091765322</v>
-      </c>
     </row>
     <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="3" t="n">
@@ -2255,12 +1373,6 @@
       <c r="B149" s="4" t="n">
         <v>42883</v>
       </c>
-      <c r="C149" s="0" t="n">
-        <v>57.3744425675675</v>
-      </c>
-      <c r="D149" s="0" t="n">
-        <v>56.2091765322</v>
-      </c>
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="3" t="n">
@@ -2269,12 +1381,6 @@
       <c r="B150" s="4" t="n">
         <v>42884</v>
       </c>
-      <c r="C150" s="0" t="n">
-        <v>57.4636549217002</v>
-      </c>
-      <c r="D150" s="0" t="n">
-        <v>56.2091765322</v>
-      </c>
     </row>
     <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="3" t="n">
@@ -2283,12 +1389,6 @@
       <c r="B151" s="4" t="n">
         <v>42885</v>
       </c>
-      <c r="C151" s="0" t="n">
-        <v>57.5541611111111</v>
-      </c>
-      <c r="D151" s="0" t="n">
-        <v>56.2091765322</v>
-      </c>
     </row>
     <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="3" t="n">
@@ -2297,12 +1397,6 @@
       <c r="B152" s="4" t="n">
         <v>42886</v>
       </c>
-      <c r="C152" s="0" t="n">
-        <v>57.6523261589404</v>
-      </c>
-      <c r="D152" s="0" t="n">
-        <v>56.2091765322</v>
-      </c>
     </row>
     <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="3" t="n">
@@ -2311,12 +1405,6 @@
       <c r="B153" s="4" t="n">
         <v>42887</v>
       </c>
-      <c r="C153" s="0" t="n">
-        <v>57.7469956140351</v>
-      </c>
-      <c r="D153" s="0" t="n">
-        <v>59.10872993</v>
-      </c>
     </row>
     <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="3" t="n">
@@ -2325,12 +1413,6 @@
       <c r="B154" s="4" t="n">
         <v>42888</v>
       </c>
-      <c r="C154" s="0" t="n">
-        <v>57.8533306100217</v>
-      </c>
-      <c r="D154" s="0" t="n">
-        <v>59.10872993</v>
-      </c>
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="3" t="n">
@@ -2339,12 +1421,6 @@
       <c r="B155" s="4" t="n">
         <v>42889</v>
       </c>
-      <c r="C155" s="0" t="n">
-        <v>57.9577272727272</v>
-      </c>
-      <c r="D155" s="0" t="n">
-        <v>59.10872993</v>
-      </c>
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="3" t="n">
@@ -2353,12 +1429,6 @@
       <c r="B156" s="4" t="n">
         <v>42890</v>
       </c>
-      <c r="C156" s="0" t="n">
-        <v>58.0508306451612</v>
-      </c>
-      <c r="D156" s="0" t="n">
-        <v>59.10872993</v>
-      </c>
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="3" t="n">
@@ -2367,12 +1437,6 @@
       <c r="B157" s="4" t="n">
         <v>42891</v>
       </c>
-      <c r="C157" s="0" t="n">
-        <v>58.1400614316239</v>
-      </c>
-      <c r="D157" s="0" t="n">
-        <v>59.10872993</v>
-      </c>
     </row>
     <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="3" t="n">
@@ -2381,12 +1445,6 @@
       <c r="B158" s="4" t="n">
         <v>42892</v>
       </c>
-      <c r="C158" s="0" t="n">
-        <v>58.2360111464968</v>
-      </c>
-      <c r="D158" s="0" t="n">
-        <v>59.10872993</v>
-      </c>
     </row>
     <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="3" t="n">
@@ -2395,12 +1453,6 @@
       <c r="B159" s="4" t="n">
         <v>42893</v>
       </c>
-      <c r="C159" s="0" t="n">
-        <v>58.312486814346</v>
-      </c>
-      <c r="D159" s="0" t="n">
-        <v>59.10872993</v>
-      </c>
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="3" t="n">
@@ -2409,12 +1461,6 @@
       <c r="B160" s="4" t="n">
         <v>42894</v>
       </c>
-      <c r="C160" s="0" t="n">
-        <v>58.3764832285115</v>
-      </c>
-      <c r="D160" s="0" t="n">
-        <v>59.10872993</v>
-      </c>
     </row>
     <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="3" t="n">
@@ -2423,12 +1469,6 @@
       <c r="B161" s="4" t="n">
         <v>42895</v>
       </c>
-      <c r="C161" s="0" t="n">
-        <v>58.4462369791666</v>
-      </c>
-      <c r="D161" s="0" t="n">
-        <v>59.10872993</v>
-      </c>
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="3" t="n">
@@ -2437,12 +1477,6 @@
       <c r="B162" s="4" t="n">
         <v>42896</v>
       </c>
-      <c r="C162" s="0" t="n">
-        <v>58.537518115942</v>
-      </c>
-      <c r="D162" s="0" t="n">
-        <v>59.10872993</v>
-      </c>
     </row>
     <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="3" t="n">
@@ -2451,12 +1485,6 @@
       <c r="B163" s="4" t="n">
         <v>42897</v>
       </c>
-      <c r="C163" s="0" t="n">
-        <v>58.6408744855967</v>
-      </c>
-      <c r="D163" s="0" t="n">
-        <v>59.10872993</v>
-      </c>
     </row>
     <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="3" t="n">
@@ -2465,12 +1493,6 @@
       <c r="B164" s="4" t="n">
         <v>42898</v>
       </c>
-      <c r="C164" s="0" t="n">
-        <v>58.7721037832311</v>
-      </c>
-      <c r="D164" s="0" t="n">
-        <v>59.10872993</v>
-      </c>
     </row>
     <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="3" t="n">
@@ -2479,12 +1501,6 @@
       <c r="B165" s="4" t="n">
         <v>42899</v>
       </c>
-      <c r="C165" s="0" t="n">
-        <v>58.8923145325203</v>
-      </c>
-      <c r="D165" s="0" t="n">
-        <v>59.10872993</v>
-      </c>
     </row>
     <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="3" t="n">
@@ -2493,12 +1509,6 @@
       <c r="B166" s="4" t="n">
         <v>42900</v>
       </c>
-      <c r="C166" s="0" t="n">
-        <v>59.0079797979798</v>
-      </c>
-      <c r="D166" s="0" t="n">
-        <v>59.10872993</v>
-      </c>
     </row>
     <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="3" t="n">
@@ -2507,12 +1517,6 @@
       <c r="B167" s="4" t="n">
         <v>42901</v>
       </c>
-      <c r="C167" s="0" t="n">
-        <v>59.1021837349397</v>
-      </c>
-      <c r="D167" s="0" t="n">
-        <v>59.10872993</v>
-      </c>
     </row>
     <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="3" t="n">
@@ -2521,12 +1525,6 @@
       <c r="B168" s="4" t="n">
         <v>42902</v>
       </c>
-      <c r="C168" s="0" t="n">
-        <v>59.1793537924151</v>
-      </c>
-      <c r="D168" s="0" t="n">
-        <v>59.10872993</v>
-      </c>
     </row>
     <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="3" t="n">
@@ -2535,12 +1533,6 @@
       <c r="B169" s="4" t="n">
         <v>42903</v>
       </c>
-      <c r="C169" s="0" t="n">
-        <v>59.2876537698412</v>
-      </c>
-      <c r="D169" s="0" t="n">
-        <v>59.10872993</v>
-      </c>
     </row>
     <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="3" t="n">
@@ -2549,12 +1541,6 @@
       <c r="B170" s="4" t="n">
         <v>42904</v>
       </c>
-      <c r="C170" s="0" t="n">
-        <v>59.3982371794871</v>
-      </c>
-      <c r="D170" s="0" t="n">
-        <v>59.10872993</v>
-      </c>
     </row>
     <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="3" t="n">
@@ -2563,12 +1549,6 @@
       <c r="B171" s="4" t="n">
         <v>42905</v>
       </c>
-      <c r="C171" s="0" t="n">
-        <v>59.4929509803921</v>
-      </c>
-      <c r="D171" s="0" t="n">
-        <v>59.10872993</v>
-      </c>
     </row>
     <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="3" t="n">
@@ -2577,12 +1557,6 @@
       <c r="B172" s="4" t="n">
         <v>42906</v>
       </c>
-      <c r="C172" s="0" t="n">
-        <v>59.5824537037037</v>
-      </c>
-      <c r="D172" s="0" t="n">
-        <v>59.10872993</v>
-      </c>
     </row>
     <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="3" t="n">
@@ -2591,12 +1565,6 @@
       <c r="B173" s="4" t="n">
         <v>42907</v>
       </c>
-      <c r="C173" s="0" t="n">
-        <v>59.6741109496124</v>
-      </c>
-      <c r="D173" s="0" t="n">
-        <v>59.10872993</v>
-      </c>
     </row>
     <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="3" t="n">
@@ -2605,12 +1573,6 @@
       <c r="B174" s="4" t="n">
         <v>42908</v>
       </c>
-      <c r="C174" s="0" t="n">
-        <v>59.7499277456647</v>
-      </c>
-      <c r="D174" s="0" t="n">
-        <v>59.10872993</v>
-      </c>
     </row>
     <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="3" t="n">
@@ -2619,12 +1581,6 @@
       <c r="B175" s="4" t="n">
         <v>42909</v>
       </c>
-      <c r="C175" s="0" t="n">
-        <v>59.849540229885</v>
-      </c>
-      <c r="D175" s="0" t="n">
-        <v>59.10872993</v>
-      </c>
     </row>
     <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="3" t="n">
@@ -2633,12 +1589,6 @@
       <c r="B176" s="4" t="n">
         <v>42910</v>
       </c>
-      <c r="C176" s="0" t="n">
-        <v>59.9535</v>
-      </c>
-      <c r="D176" s="0" t="n">
-        <v>59.10872993</v>
-      </c>
     </row>
     <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="3" t="n">
@@ -2647,12 +1597,6 @@
       <c r="B177" s="4" t="n">
         <v>42911</v>
       </c>
-      <c r="C177" s="0" t="n">
-        <v>60.0144223484848</v>
-      </c>
-      <c r="D177" s="0" t="n">
-        <v>59.10872993</v>
-      </c>
     </row>
     <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="3" t="n">
@@ -2661,12 +1605,6 @@
       <c r="B178" s="4" t="n">
         <v>42912</v>
       </c>
-      <c r="C178" s="0" t="n">
-        <v>60.0699223163841</v>
-      </c>
-      <c r="D178" s="0" t="n">
-        <v>59.10872993</v>
-      </c>
     </row>
     <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="3" t="n">
@@ -2675,12 +1613,6 @@
       <c r="B179" s="4" t="n">
         <v>42913</v>
       </c>
-      <c r="C179" s="0" t="n">
-        <v>60.1299227528089</v>
-      </c>
-      <c r="D179" s="0" t="n">
-        <v>59.10872993</v>
-      </c>
     </row>
     <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="3" t="n">
@@ -2689,12 +1621,6 @@
       <c r="B180" s="4" t="n">
         <v>42914</v>
       </c>
-      <c r="C180" s="0" t="n">
-        <v>60.192418528864</v>
-      </c>
-      <c r="D180" s="0" t="n">
-        <v>59.10872993</v>
-      </c>
     </row>
     <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="3" t="n">
@@ -2703,12 +1629,6 @@
       <c r="B181" s="4" t="n">
         <v>42915</v>
       </c>
-      <c r="C181" s="0" t="n">
-        <v>60.2672777777777</v>
-      </c>
-      <c r="D181" s="0" t="n">
-        <v>59.10872993</v>
-      </c>
     </row>
     <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="3" t="n">
@@ -2717,12 +1637,6 @@
       <c r="B182" s="4" t="n">
         <v>42916</v>
       </c>
-      <c r="C182" s="0" t="n">
-        <v>60.3470695211786</v>
-      </c>
-      <c r="D182" s="0" t="n">
-        <v>59.10872993</v>
-      </c>
     </row>
     <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="3" t="n">
@@ -2731,12 +1645,6 @@
       <c r="B183" s="4" t="n">
         <v>42917</v>
       </c>
-      <c r="C183" s="0" t="n">
-        <v>60.4344688644688</v>
-      </c>
-      <c r="D183" s="0" t="n">
-        <v>61.718225334</v>
-      </c>
     </row>
     <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="3" t="n">
@@ -2745,12 +1653,6 @@
       <c r="B184" s="4" t="n">
         <v>42918</v>
       </c>
-      <c r="C184" s="0" t="n">
-        <v>60.5063820582877</v>
-      </c>
-      <c r="D184" s="0" t="n">
-        <v>61.718225334</v>
-      </c>
     </row>
     <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="3" t="n">
@@ -2759,12 +1661,6 @@
       <c r="B185" s="4" t="n">
         <v>42919</v>
       </c>
-      <c r="C185" s="0" t="n">
-        <v>60.5932133152174</v>
-      </c>
-      <c r="D185" s="0" t="n">
-        <v>61.718225334</v>
-      </c>
     </row>
     <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="3" t="n">
@@ -2773,12 +1669,6 @@
       <c r="B186" s="4" t="n">
         <v>42920</v>
       </c>
-      <c r="C186" s="0" t="n">
-        <v>60.670295045045</v>
-      </c>
-      <c r="D186" s="0" t="n">
-        <v>61.718225334</v>
-      </c>
     </row>
     <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="3" t="n">
@@ -2787,12 +1677,6 @@
       <c r="B187" s="4" t="n">
         <v>42921</v>
       </c>
-      <c r="C187" s="0" t="n">
-        <v>60.7528741039426</v>
-      </c>
-      <c r="D187" s="0" t="n">
-        <v>61.718225334</v>
-      </c>
     </row>
     <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="3" t="n">
@@ -2801,12 +1685,6 @@
       <c r="B188" s="4" t="n">
         <v>42922</v>
       </c>
-      <c r="C188" s="0" t="n">
-        <v>60.8296100713012</v>
-      </c>
-      <c r="D188" s="0" t="n">
-        <v>61.718225334</v>
-      </c>
     </row>
     <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="3" t="n">
@@ -2815,12 +1693,6 @@
       <c r="B189" s="4" t="n">
         <v>42923</v>
       </c>
-      <c r="C189" s="0" t="n">
-        <v>60.9172052304964</v>
-      </c>
-      <c r="D189" s="0" t="n">
-        <v>61.718225334</v>
-      </c>
     </row>
     <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="3" t="n">
@@ -2829,12 +1701,6 @@
       <c r="B190" s="4" t="n">
         <v>42924</v>
       </c>
-      <c r="C190" s="0" t="n">
-        <v>61.0045105820105</v>
-      </c>
-      <c r="D190" s="0" t="n">
-        <v>61.718225334</v>
-      </c>
     </row>
     <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="3" t="n">
@@ -2843,12 +1709,6 @@
       <c r="B191" s="4" t="n">
         <v>42925</v>
       </c>
-      <c r="C191" s="0" t="n">
-        <v>61.087596491228</v>
-      </c>
-      <c r="D191" s="0" t="n">
-        <v>61.718225334</v>
-      </c>
     </row>
     <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="3" t="n">
@@ -2857,12 +1717,6 @@
       <c r="B192" s="4" t="n">
         <v>42926</v>
       </c>
-      <c r="C192" s="0" t="n">
-        <v>61.1690423211169</v>
-      </c>
-      <c r="D192" s="0" t="n">
-        <v>61.718225334</v>
-      </c>
     </row>
     <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="3" t="n">
@@ -2871,12 +1725,6 @@
       <c r="B193" s="4" t="n">
         <v>42927</v>
       </c>
-      <c r="C193" s="0" t="n">
-        <v>61.2577517361111</v>
-      </c>
-      <c r="D193" s="0" t="n">
-        <v>61.718225334</v>
-      </c>
     </row>
     <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="3" t="n">
@@ -2885,12 +1733,6 @@
       <c r="B194" s="4" t="n">
         <v>42928</v>
       </c>
-      <c r="C194" s="0" t="n">
-        <v>61.3536938687391</v>
-      </c>
-      <c r="D194" s="0" t="n">
-        <v>61.718225334</v>
-      </c>
     </row>
     <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="3" t="n">
@@ -2899,12 +1741,6 @@
       <c r="B195" s="4" t="n">
         <v>42929</v>
       </c>
-      <c r="C195" s="0" t="n">
-        <v>61.4566602233676</v>
-      </c>
-      <c r="D195" s="0" t="n">
-        <v>61.718225334</v>
-      </c>
     </row>
     <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="3" t="n">
@@ -2913,12 +1749,6 @@
       <c r="B196" s="4" t="n">
         <v>42930</v>
       </c>
-      <c r="C196" s="0" t="n">
-        <v>61.546267094017</v>
-      </c>
-      <c r="D196" s="0" t="n">
-        <v>61.718225334</v>
-      </c>
     </row>
     <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="3" t="n">
@@ -2927,12 +1757,6 @@
       <c r="B197" s="4" t="n">
         <v>42931</v>
       </c>
-      <c r="C197" s="0" t="n">
-        <v>61.6167495748299</v>
-      </c>
-      <c r="D197" s="0" t="n">
-        <v>61.718225334</v>
-      </c>
     </row>
     <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="3" t="n">
@@ -2941,12 +1765,6 @@
       <c r="B198" s="4" t="n">
         <v>42932</v>
       </c>
-      <c r="C198" s="0" t="n">
-        <v>61.6958989001691</v>
-      </c>
-      <c r="D198" s="0" t="n">
-        <v>61.718225334</v>
-      </c>
     </row>
     <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="3" t="n">
@@ -2955,12 +1773,6 @@
       <c r="B199" s="4" t="n">
         <v>42933</v>
       </c>
-      <c r="C199" s="0" t="n">
-        <v>61.7828177609427</v>
-      </c>
-      <c r="D199" s="0" t="n">
-        <v>61.718225334</v>
-      </c>
     </row>
     <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="3" t="n">
@@ -2969,12 +1781,6 @@
       <c r="B200" s="4" t="n">
         <v>42934</v>
       </c>
-      <c r="C200" s="0" t="n">
-        <v>61.8633605527637</v>
-      </c>
-      <c r="D200" s="0" t="n">
-        <v>61.718225334</v>
-      </c>
     </row>
     <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="3" t="n">
@@ -2983,12 +1789,6 @@
       <c r="B201" s="4" t="n">
         <v>42935</v>
       </c>
-      <c r="C201" s="0" t="n">
-        <v>61.9587770833332</v>
-      </c>
-      <c r="D201" s="0" t="n">
-        <v>61.718225334</v>
-      </c>
     </row>
     <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="3" t="n">
@@ -2997,12 +1797,6 @@
       <c r="B202" s="4" t="n">
         <v>42936</v>
       </c>
-      <c r="C202" s="0" t="n">
-        <v>62.0547616086235</v>
-      </c>
-      <c r="D202" s="0" t="n">
-        <v>61.718225334</v>
-      </c>
     </row>
     <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="3" t="n">
@@ -3011,12 +1805,6 @@
       <c r="B203" s="4" t="n">
         <v>42937</v>
       </c>
-      <c r="C203" s="0" t="n">
-        <v>62.15963490099</v>
-      </c>
-      <c r="D203" s="0" t="n">
-        <v>61.718225334</v>
-      </c>
     </row>
     <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="3" t="n">
@@ -3025,12 +1813,6 @@
       <c r="B204" s="4" t="n">
         <v>42938</v>
       </c>
-      <c r="C204" s="0" t="n">
-        <v>62.2694868637109</v>
-      </c>
-      <c r="D204" s="0" t="n">
-        <v>61.718225334</v>
-      </c>
     </row>
     <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="3" t="n">
@@ -3039,12 +1821,6 @@
       <c r="B205" s="4" t="n">
         <v>42939</v>
       </c>
-      <c r="C205" s="0" t="n">
-        <v>62.3674918300653</v>
-      </c>
-      <c r="D205" s="0" t="n">
-        <v>61.718225334</v>
-      </c>
     </row>
     <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="3" t="n">
@@ -3053,12 +1829,6 @@
       <c r="B206" s="4" t="n">
         <v>42940</v>
       </c>
-      <c r="C206" s="0" t="n">
-        <v>62.455231707317</v>
-      </c>
-      <c r="D206" s="0" t="n">
-        <v>61.718225334</v>
-      </c>
     </row>
     <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="3" t="n">
@@ -3067,12 +1837,6 @@
       <c r="B207" s="4" t="n">
         <v>42941</v>
       </c>
-      <c r="C207" s="0" t="n">
-        <v>62.5450303398058</v>
-      </c>
-      <c r="D207" s="0" t="n">
-        <v>61.718225334</v>
-      </c>
     </row>
     <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="3" t="n">
@@ -3081,12 +1845,6 @@
       <c r="B208" s="4" t="n">
         <v>42942</v>
       </c>
-      <c r="C208" s="0" t="n">
-        <v>62.6386735104669</v>
-      </c>
-      <c r="D208" s="0" t="n">
-        <v>61.718225334</v>
-      </c>
     </row>
     <row r="209" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="3" t="n">
@@ -3095,12 +1853,6 @@
       <c r="B209" s="4" t="n">
         <v>42943</v>
       </c>
-      <c r="C209" s="0" t="n">
-        <v>62.7292067307692</v>
-      </c>
-      <c r="D209" s="0" t="n">
-        <v>61.718225334</v>
-      </c>
     </row>
     <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="3" t="n">
@@ -3109,12 +1861,6 @@
       <c r="B210" s="4" t="n">
         <v>42944</v>
       </c>
-      <c r="C210" s="0" t="n">
-        <v>62.7936602870813</v>
-      </c>
-      <c r="D210" s="0" t="n">
-        <v>61.718225334</v>
-      </c>
     </row>
     <row r="211" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="3" t="n">
@@ -3123,12 +1869,6 @@
       <c r="B211" s="4" t="n">
         <v>42945</v>
       </c>
-      <c r="C211" s="0" t="n">
-        <v>62.8617817460317</v>
-      </c>
-      <c r="D211" s="0" t="n">
-        <v>61.718225334</v>
-      </c>
     </row>
     <row r="212" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="3" t="n">
@@ -3137,12 +1877,6 @@
       <c r="B212" s="4" t="n">
         <v>42946</v>
       </c>
-      <c r="C212" s="0" t="n">
-        <v>62.9185683254343</v>
-      </c>
-      <c r="D212" s="0" t="n">
-        <v>61.718225334</v>
-      </c>
     </row>
     <row r="213" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="3" t="n">
@@ -3151,12 +1885,6 @@
       <c r="B213" s="4" t="n">
         <v>42947</v>
       </c>
-      <c r="C213" s="0" t="n">
-        <v>62.9742826257861</v>
-      </c>
-      <c r="D213" s="0" t="n">
-        <v>61.718225334</v>
-      </c>
     </row>
     <row r="214" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="3" t="n">
@@ -3165,12 +1893,6 @@
       <c r="B214" s="4" t="n">
         <v>42948</v>
       </c>
-      <c r="C214" s="0" t="n">
-        <v>63.0309448356807</v>
-      </c>
-      <c r="D214" s="0" t="n">
-        <v>63.9121630163</v>
-      </c>
     </row>
     <row r="215" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="3" t="n">
@@ -3179,12 +1901,6 @@
       <c r="B215" s="4" t="n">
         <v>42949</v>
       </c>
-      <c r="C215" s="0" t="n">
-        <v>63.0933781152647</v>
-      </c>
-      <c r="D215" s="0" t="n">
-        <v>63.9121630163</v>
-      </c>
     </row>
     <row r="216" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="3" t="n">
@@ -3193,12 +1909,6 @@
       <c r="B216" s="4" t="n">
         <v>42950</v>
       </c>
-      <c r="C216" s="0" t="n">
-        <v>63.1529670542635</v>
-      </c>
-      <c r="D216" s="0" t="n">
-        <v>63.9121630163</v>
-      </c>
     </row>
     <row r="217" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="3" t="n">
@@ -3207,12 +1917,6 @@
       <c r="B217" s="4" t="n">
         <v>42951</v>
       </c>
-      <c r="C217" s="0" t="n">
-        <v>63.2208449074073</v>
-      </c>
-      <c r="D217" s="0" t="n">
-        <v>63.9121630163</v>
-      </c>
     </row>
     <row r="218" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="3" t="n">
@@ -3221,12 +1925,6 @@
       <c r="B218" s="4" t="n">
         <v>42952</v>
       </c>
-      <c r="C218" s="0" t="n">
-        <v>63.2707027649769</v>
-      </c>
-      <c r="D218" s="0" t="n">
-        <v>63.9121630163</v>
-      </c>
     </row>
     <row r="219" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="3" t="n">
@@ -3235,12 +1933,6 @@
       <c r="B219" s="4" t="n">
         <v>42953</v>
       </c>
-      <c r="C219" s="0" t="n">
-        <v>63.3162595565748</v>
-      </c>
-      <c r="D219" s="0" t="n">
-        <v>63.9121630163</v>
-      </c>
     </row>
     <row r="220" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="3" t="n">
@@ -3249,12 +1941,6 @@
       <c r="B220" s="4" t="n">
         <v>42954</v>
       </c>
-      <c r="C220" s="0" t="n">
-        <v>63.3666419330288</v>
-      </c>
-      <c r="D220" s="0" t="n">
-        <v>63.9121630163</v>
-      </c>
     </row>
     <row r="221" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="3" t="n">
@@ -3263,12 +1949,6 @@
       <c r="B221" s="4" t="n">
         <v>42955</v>
       </c>
-      <c r="C221" s="0" t="n">
-        <v>63.4222405303029</v>
-      </c>
-      <c r="D221" s="0" t="n">
-        <v>63.9121630163</v>
-      </c>
     </row>
     <row r="222" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="3" t="n">
@@ -3277,12 +1957,6 @@
       <c r="B222" s="4" t="n">
         <v>42956</v>
       </c>
-      <c r="C222" s="0" t="n">
-        <v>63.4738932880844</v>
-      </c>
-      <c r="D222" s="0" t="n">
-        <v>63.9121630163</v>
-      </c>
     </row>
     <row r="223" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="3" t="n">
@@ -3291,12 +1965,6 @@
       <c r="B223" s="4" t="n">
         <v>42957</v>
       </c>
-      <c r="C223" s="0" t="n">
-        <v>63.5264677177176</v>
-      </c>
-      <c r="D223" s="0" t="n">
-        <v>63.9121630163</v>
-      </c>
     </row>
     <row r="224" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="3" t="n">
@@ -3305,12 +1973,6 @@
       <c r="B224" s="4" t="n">
         <v>42958</v>
       </c>
-      <c r="C224" s="0" t="n">
-        <v>63.5862257100149</v>
-      </c>
-      <c r="D224" s="0" t="n">
-        <v>63.9121630163</v>
-      </c>
     </row>
     <row r="225" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="3" t="n">
@@ -3319,12 +1981,6 @@
       <c r="B225" s="4" t="n">
         <v>42959</v>
       </c>
-      <c r="C225" s="0" t="n">
-        <v>63.6549795386904</v>
-      </c>
-      <c r="D225" s="0" t="n">
-        <v>63.9121630163</v>
-      </c>
     </row>
     <row r="226" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="3" t="n">
@@ -3333,12 +1989,6 @@
       <c r="B226" s="4" t="n">
         <v>42960</v>
       </c>
-      <c r="C226" s="0" t="n">
-        <v>63.7155944444443</v>
-      </c>
-      <c r="D226" s="0" t="n">
-        <v>63.9121630163</v>
-      </c>
     </row>
     <row r="227" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="3" t="n">
@@ -3347,12 +1997,6 @@
       <c r="B227" s="4" t="n">
         <v>42961</v>
       </c>
-      <c r="C227" s="0" t="n">
-        <v>63.7765099557521</v>
-      </c>
-      <c r="D227" s="0" t="n">
-        <v>63.9121630163</v>
-      </c>
     </row>
     <row r="228" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="3" t="n">
@@ -3361,12 +2005,6 @@
       <c r="B228" s="4" t="n">
         <v>42962</v>
       </c>
-      <c r="C228" s="0" t="n">
-        <v>63.8454588839941</v>
-      </c>
-      <c r="D228" s="0" t="n">
-        <v>63.9121630163</v>
-      </c>
     </row>
     <row r="229" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="3" t="n">
@@ -3375,12 +2013,6 @@
       <c r="B229" s="4" t="n">
         <v>42963</v>
       </c>
-      <c r="C229" s="0" t="n">
-        <v>63.9156304824561</v>
-      </c>
-      <c r="D229" s="0" t="n">
-        <v>63.9121630163</v>
-      </c>
     </row>
     <row r="230" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="3" t="n">
@@ -3389,12 +2021,6 @@
       <c r="B230" s="4" t="n">
         <v>42964</v>
       </c>
-      <c r="C230" s="0" t="n">
-        <v>63.9917339883551</v>
-      </c>
-      <c r="D230" s="0" t="n">
-        <v>63.9121630163</v>
-      </c>
     </row>
     <row r="231" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="3" t="n">
@@ -3403,12 +2029,6 @@
       <c r="B231" s="4" t="n">
         <v>42965</v>
       </c>
-      <c r="C231" s="0" t="n">
-        <v>64.0664963768115</v>
-      </c>
-      <c r="D231" s="0" t="n">
-        <v>63.9121630163</v>
-      </c>
     </row>
     <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="3" t="n">
@@ -3417,12 +2037,6 @@
       <c r="B232" s="4" t="n">
         <v>42966</v>
       </c>
-      <c r="C232" s="0" t="n">
-        <v>64.1246121933621</v>
-      </c>
-      <c r="D232" s="0" t="n">
-        <v>63.9121630163</v>
-      </c>
     </row>
     <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="3" t="n">
@@ -3431,12 +2045,6 @@
       <c r="B233" s="4" t="n">
         <v>42967</v>
       </c>
-      <c r="C233" s="0" t="n">
-        <v>64.1894899425287</v>
-      </c>
-      <c r="D233" s="0" t="n">
-        <v>63.9121630163</v>
-      </c>
     </row>
     <row r="234" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="3" t="n">
@@ -3445,12 +2053,6 @@
       <c r="B234" s="4" t="n">
         <v>42968</v>
       </c>
-      <c r="C234" s="0" t="n">
-        <v>64.2575321888411</v>
-      </c>
-      <c r="D234" s="0" t="n">
-        <v>63.9121630163</v>
-      </c>
     </row>
     <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="3" t="n">
@@ -3459,12 +2061,6 @@
       <c r="B235" s="4" t="n">
         <v>42969</v>
       </c>
-      <c r="C235" s="0" t="n">
-        <v>64.3298646723646</v>
-      </c>
-      <c r="D235" s="0" t="n">
-        <v>63.9121630163</v>
-      </c>
     </row>
     <row r="236" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="3" t="n">
@@ -3473,12 +2069,6 @@
       <c r="B236" s="4" t="n">
         <v>42970</v>
       </c>
-      <c r="C236" s="0" t="n">
-        <v>64.3960833333333</v>
-      </c>
-      <c r="D236" s="0" t="n">
-        <v>63.9121630163</v>
-      </c>
     </row>
     <row r="237" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="3" t="n">
@@ -3487,12 +2077,6 @@
       <c r="B237" s="4" t="n">
         <v>42971</v>
       </c>
-      <c r="C237" s="0" t="n">
-        <v>64.4355808615819</v>
-      </c>
-      <c r="D237" s="0" t="n">
-        <v>63.9121630163</v>
-      </c>
     </row>
     <row r="238" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="3" t="n">
@@ -3501,12 +2085,6 @@
       <c r="B238" s="4" t="n">
         <v>42972</v>
       </c>
-      <c r="C238" s="0" t="n">
-        <v>64.4714486638537</v>
-      </c>
-      <c r="D238" s="0" t="n">
-        <v>63.9121630163</v>
-      </c>
     </row>
     <row r="239" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="3" t="n">
@@ -3515,12 +2093,6 @@
       <c r="B239" s="4" t="n">
         <v>42973</v>
       </c>
-      <c r="C239" s="0" t="n">
-        <v>64.5136782212884</v>
-      </c>
-      <c r="D239" s="0" t="n">
-        <v>63.9121630163</v>
-      </c>
     </row>
     <row r="240" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="3" t="n">
@@ -3529,12 +2101,6 @@
       <c r="B240" s="4" t="n">
         <v>42974</v>
       </c>
-      <c r="C240" s="0" t="n">
-        <v>64.5612726638772</v>
-      </c>
-      <c r="D240" s="0" t="n">
-        <v>63.9121630163</v>
-      </c>
     </row>
     <row r="241" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="3" t="n">
@@ -3543,12 +2109,6 @@
       <c r="B241" s="4" t="n">
         <v>42975</v>
       </c>
-      <c r="C241" s="0" t="n">
-        <v>64.5949565972221</v>
-      </c>
-      <c r="D241" s="0" t="n">
-        <v>63.9121630163</v>
-      </c>
     </row>
     <row r="242" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="3" t="n">
@@ -3557,12 +2117,6 @@
       <c r="B242" s="4" t="n">
         <v>42976</v>
       </c>
-      <c r="C242" s="0" t="n">
-        <v>64.6319917012447</v>
-      </c>
-      <c r="D242" s="0" t="n">
-        <v>63.9121630163</v>
-      </c>
     </row>
     <row r="243" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="3" t="n">
@@ -3571,12 +2125,6 @@
       <c r="B243" s="4" t="n">
         <v>42977</v>
       </c>
-      <c r="C243" s="0" t="n">
-        <v>64.6589221763084</v>
-      </c>
-      <c r="D243" s="0" t="n">
-        <v>63.9121630163</v>
-      </c>
     </row>
     <row r="244" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="3" t="n">
@@ -3585,12 +2133,6 @@
       <c r="B244" s="4" t="n">
         <v>42978</v>
       </c>
-      <c r="C244" s="0" t="n">
-        <v>64.6846502057612</v>
-      </c>
-      <c r="D244" s="0" t="n">
-        <v>63.9121630163</v>
-      </c>
     </row>
     <row r="245" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="3" t="n">
@@ -3599,12 +2141,6 @@
       <c r="B245" s="4" t="n">
         <v>42979</v>
       </c>
-      <c r="C245" s="0" t="n">
-        <v>64.7116956967212</v>
-      </c>
-      <c r="D245" s="0" t="n">
-        <v>64.9023712925</v>
-      </c>
     </row>
     <row r="246" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="3" t="n">
@@ -3613,12 +2149,6 @@
       <c r="B246" s="4" t="n">
         <v>42980</v>
       </c>
-      <c r="C246" s="0" t="n">
-        <v>64.7209387755101</v>
-      </c>
-      <c r="D246" s="0" t="n">
-        <v>64.9023712925</v>
-      </c>
     </row>
     <row r="247" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="3" t="n">
@@ -3627,12 +2157,6 @@
       <c r="B247" s="4" t="n">
         <v>42981</v>
       </c>
-      <c r="C247" s="0" t="n">
-        <v>64.734127710027</v>
-      </c>
-      <c r="D247" s="0" t="n">
-        <v>64.9023712925</v>
-      </c>
     </row>
     <row r="248" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="3" t="n">
@@ -3641,12 +2165,6 @@
       <c r="B248" s="4" t="n">
         <v>42982</v>
       </c>
-      <c r="C248" s="0" t="n">
-        <v>64.7611757759783</v>
-      </c>
-      <c r="D248" s="0" t="n">
-        <v>64.9023712925</v>
-      </c>
     </row>
     <row r="249" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="3" t="n">
@@ -3655,12 +2173,6 @@
       <c r="B249" s="4" t="n">
         <v>42983</v>
       </c>
-      <c r="C249" s="0" t="n">
-        <v>64.7854267473117</v>
-      </c>
-      <c r="D249" s="0" t="n">
-        <v>64.9023712925</v>
-      </c>
     </row>
     <row r="250" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="3" t="n">
@@ -3669,12 +2181,6 @@
       <c r="B250" s="4" t="n">
         <v>42984</v>
       </c>
-      <c r="C250" s="0" t="n">
-        <v>64.7920665997322</v>
-      </c>
-      <c r="D250" s="0" t="n">
-        <v>64.9023712925</v>
-      </c>
     </row>
     <row r="251" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="3" t="n">
@@ -3683,12 +2189,6 @@
       <c r="B251" s="4" t="n">
         <v>42985</v>
       </c>
-      <c r="C251" s="0" t="n">
-        <v>64.7783549999999</v>
-      </c>
-      <c r="D251" s="0" t="n">
-        <v>64.9023712925</v>
-      </c>
     </row>
     <row r="252" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="3" t="n">
@@ -3697,12 +2197,6 @@
       <c r="B252" s="4" t="n">
         <v>42986</v>
       </c>
-      <c r="C252" s="0" t="n">
-        <v>64.7731839309428</v>
-      </c>
-      <c r="D252" s="0" t="n">
-        <v>64.9023712925</v>
-      </c>
     </row>
     <row r="253" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="3" t="n">
@@ -3711,12 +2205,6 @@
       <c r="B253" s="4" t="n">
         <v>42987</v>
       </c>
-      <c r="C253" s="0" t="n">
-        <v>64.7804100529099</v>
-      </c>
-      <c r="D253" s="0" t="n">
-        <v>64.9023712925</v>
-      </c>
     </row>
     <row r="254" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="3" t="n">
@@ -3725,12 +2213,6 @@
       <c r="B254" s="4" t="n">
         <v>42988</v>
       </c>
-      <c r="C254" s="0" t="n">
-        <v>64.7875625823451</v>
-      </c>
-      <c r="D254" s="0" t="n">
-        <v>64.9023712925</v>
-      </c>
     </row>
     <row r="255" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="3" t="n">
@@ -3739,12 +2221,6 @@
       <c r="B255" s="4" t="n">
         <v>42989</v>
       </c>
-      <c r="C255" s="0" t="n">
-        <v>64.7666289370077</v>
-      </c>
-      <c r="D255" s="0" t="n">
-        <v>64.9023712925</v>
-      </c>
     </row>
     <row r="256" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="3" t="n">
@@ -3753,12 +2229,6 @@
       <c r="B256" s="4" t="n">
         <v>42990</v>
       </c>
-      <c r="C256" s="0" t="n">
-        <v>64.7526683006535</v>
-      </c>
-      <c r="D256" s="0" t="n">
-        <v>64.9023712925</v>
-      </c>
     </row>
     <row r="257" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="3" t="n">
@@ -3767,12 +2237,6 @@
       <c r="B257" s="4" t="n">
         <v>42991</v>
       </c>
-      <c r="C257" s="0" t="n">
-        <v>64.7406119791665</v>
-      </c>
-      <c r="D257" s="0" t="n">
-        <v>64.9023712925</v>
-      </c>
     </row>
     <row r="258" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="3" t="n">
@@ -3781,12 +2245,6 @@
       <c r="B258" s="4" t="n">
         <v>42992</v>
       </c>
-      <c r="C258" s="0" t="n">
-        <v>64.7509079118027</v>
-      </c>
-      <c r="D258" s="0" t="n">
-        <v>64.9023712925</v>
-      </c>
     </row>
     <row r="259" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="3" t="n">
@@ -3795,12 +2253,6 @@
       <c r="B259" s="4" t="n">
         <v>42993</v>
       </c>
-      <c r="C259" s="0" t="n">
-        <v>64.772905361757</v>
-      </c>
-      <c r="D259" s="0" t="n">
-        <v>64.9023712925</v>
-      </c>
     </row>
     <row r="260" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="3" t="n">
@@ -3809,12 +2261,6 @@
       <c r="B260" s="4" t="n">
         <v>42994</v>
       </c>
-      <c r="C260" s="0" t="n">
-        <v>64.801319176319</v>
-      </c>
-      <c r="D260" s="0" t="n">
-        <v>64.9023712925</v>
-      </c>
     </row>
     <row r="261" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="3" t="n">
@@ -3823,12 +2269,6 @@
       <c r="B261" s="4" t="n">
         <v>42995</v>
       </c>
-      <c r="C261" s="0" t="n">
-        <v>64.8345929487178</v>
-      </c>
-      <c r="D261" s="0" t="n">
-        <v>64.9023712925</v>
-      </c>
     </row>
     <row r="262" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="3" t="n">
@@ -3837,12 +2277,6 @@
       <c r="B262" s="4" t="n">
         <v>42996</v>
       </c>
-      <c r="C262" s="0" t="n">
-        <v>64.8683253512131</v>
-      </c>
-      <c r="D262" s="0" t="n">
-        <v>64.9023712925</v>
-      </c>
     </row>
     <row r="263" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="3" t="n">
@@ -3851,12 +2285,6 @@
       <c r="B263" s="4" t="n">
         <v>42997</v>
       </c>
-      <c r="C263" s="0" t="n">
-        <v>64.8927194656487</v>
-      </c>
-      <c r="D263" s="0" t="n">
-        <v>64.9023712925</v>
-      </c>
     </row>
     <row r="264" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="3" t="n">
@@ -3865,12 +2293,6 @@
       <c r="B264" s="4" t="n">
         <v>42998</v>
       </c>
-      <c r="C264" s="0" t="n">
-        <v>64.9252645754118</v>
-      </c>
-      <c r="D264" s="0" t="n">
-        <v>64.9023712925</v>
-      </c>
     </row>
     <row r="265" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="3" t="n">
@@ -3879,12 +2301,6 @@
       <c r="B265" s="4" t="n">
         <v>42999</v>
       </c>
-      <c r="C265" s="0" t="n">
-        <v>64.9673595328281</v>
-      </c>
-      <c r="D265" s="0" t="n">
-        <v>64.9023712925</v>
-      </c>
     </row>
     <row r="266" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="3" t="n">
@@ -3893,12 +2309,6 @@
       <c r="B266" s="4" t="n">
         <v>43000</v>
       </c>
-      <c r="C266" s="0" t="n">
-        <v>65.0082704402514</v>
-      </c>
-      <c r="D266" s="0" t="n">
-        <v>64.9023712925</v>
-      </c>
     </row>
     <row r="267" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="3" t="n">
@@ -3907,12 +2317,6 @@
       <c r="B267" s="4" t="n">
         <v>43001</v>
       </c>
-      <c r="C267" s="0" t="n">
-        <v>65.0503117167918</v>
-      </c>
-      <c r="D267" s="0" t="n">
-        <v>64.9023712925</v>
-      </c>
     </row>
     <row r="268" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="3" t="n">
@@ -3921,12 +2325,6 @@
       <c r="B268" s="4" t="n">
         <v>43002</v>
       </c>
-      <c r="C268" s="0" t="n">
-        <v>65.0872737203494</v>
-      </c>
-      <c r="D268" s="0" t="n">
-        <v>64.9023712925</v>
-      </c>
     </row>
     <row r="269" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="3" t="n">
@@ -3935,12 +2333,6 @@
       <c r="B269" s="4" t="n">
         <v>43003</v>
       </c>
-      <c r="C269" s="0" t="n">
-        <v>65.123205845771</v>
-      </c>
-      <c r="D269" s="0" t="n">
-        <v>64.9023712925</v>
-      </c>
     </row>
     <row r="270" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="3" t="n">
@@ -3949,12 +2341,6 @@
       <c r="B270" s="4" t="n">
         <v>43004</v>
       </c>
-      <c r="C270" s="0" t="n">
-        <v>65.1566883519205</v>
-      </c>
-      <c r="D270" s="0" t="n">
-        <v>64.9023712925</v>
-      </c>
     </row>
     <row r="271" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="3" t="n">
@@ -3963,12 +2349,6 @@
       <c r="B271" s="4" t="n">
         <v>43005</v>
       </c>
-      <c r="C271" s="0" t="n">
-        <v>65.1945771604937</v>
-      </c>
-      <c r="D271" s="0" t="n">
-        <v>64.9023712925</v>
-      </c>
     </row>
     <row r="272" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="3" t="n">
@@ -3977,12 +2357,6 @@
       <c r="B272" s="4" t="n">
         <v>43006</v>
       </c>
-      <c r="C272" s="0" t="n">
-        <v>65.2303582410823</v>
-      </c>
-      <c r="D272" s="0" t="n">
-        <v>64.9023712925</v>
-      </c>
     </row>
     <row r="273" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="3" t="n">
@@ -3991,12 +2365,6 @@
       <c r="B273" s="4" t="n">
         <v>43007</v>
       </c>
-      <c r="C273" s="0" t="n">
-        <v>65.2549800857842</v>
-      </c>
-      <c r="D273" s="0" t="n">
-        <v>64.9023712925</v>
-      </c>
     </row>
     <row r="274" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A274" s="3" t="n">
@@ -4005,12 +2373,6 @@
       <c r="B274" s="4" t="n">
         <v>43008</v>
       </c>
-      <c r="C274" s="0" t="n">
-        <v>65.2672268009767</v>
-      </c>
-      <c r="D274" s="0" t="n">
-        <v>64.9023712925</v>
-      </c>
     </row>
     <row r="275" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="3" t="n">
@@ -4019,12 +2381,6 @@
       <c r="B275" s="4" t="n">
         <v>43009</v>
       </c>
-      <c r="C275" s="0" t="n">
-        <v>65.2620498783454</v>
-      </c>
-      <c r="D275" s="0" t="n">
-        <v>65.3262645397</v>
-      </c>
     </row>
     <row r="276" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="3" t="n">
@@ -4033,12 +2389,6 @@
       <c r="B276" s="4" t="n">
         <v>43010</v>
       </c>
-      <c r="C276" s="0" t="n">
-        <v>65.2554439393938</v>
-      </c>
-      <c r="D276" s="0" t="n">
-        <v>65.3262645397</v>
-      </c>
     </row>
     <row r="277" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="3" t="n">
@@ -4047,12 +2397,6 @@
       <c r="B277" s="4" t="n">
         <v>43011</v>
       </c>
-      <c r="C277" s="0" t="n">
-        <v>65.2645003019322</v>
-      </c>
-      <c r="D277" s="0" t="n">
-        <v>65.3262645397</v>
-      </c>
     </row>
     <row r="278" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="3" t="n">
@@ -4061,12 +2405,6 @@
       <c r="B278" s="4" t="n">
         <v>43012</v>
       </c>
-      <c r="C278" s="0" t="n">
-        <v>65.2726293622141</v>
-      </c>
-      <c r="D278" s="0" t="n">
-        <v>65.3262645397</v>
-      </c>
     </row>
     <row r="279" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="3" t="n">
@@ -4075,12 +2413,6 @@
       <c r="B279" s="4" t="n">
         <v>43013</v>
       </c>
-      <c r="C279" s="0" t="n">
-        <v>65.2806249999999</v>
-      </c>
-      <c r="D279" s="0" t="n">
-        <v>65.3262645397</v>
-      </c>
     </row>
     <row r="280" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="3" t="n">
@@ -4089,12 +2421,6 @@
       <c r="B280" s="4" t="n">
         <v>43014</v>
       </c>
-      <c r="C280" s="0" t="n">
-        <v>65.2929674432496</v>
-      </c>
-      <c r="D280" s="0" t="n">
-        <v>65.3262645397</v>
-      </c>
     </row>
     <row r="281" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="3" t="n">
@@ -4103,12 +2429,6 @@
       <c r="B281" s="4" t="n">
         <v>43015</v>
       </c>
-      <c r="C281" s="0" t="n">
-        <v>65.3189241071427</v>
-      </c>
-      <c r="D281" s="0" t="n">
-        <v>65.3262645397</v>
-      </c>
     </row>
     <row r="282" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="3" t="n">
@@ -4117,12 +2437,6 @@
       <c r="B282" s="4" t="n">
         <v>43016</v>
       </c>
-      <c r="C282" s="0" t="n">
-        <v>65.3440332147092</v>
-      </c>
-      <c r="D282" s="0" t="n">
-        <v>65.3262645397</v>
-      </c>
     </row>
     <row r="283" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A283" s="3" t="n">
@@ -4131,12 +2445,6 @@
       <c r="B283" s="4" t="n">
         <v>43017</v>
       </c>
-      <c r="C283" s="0" t="n">
-        <v>65.38367464539</v>
-      </c>
-      <c r="D283" s="0" t="n">
-        <v>65.3262645397</v>
-      </c>
     </row>
     <row r="284" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="3" t="n">
@@ -4145,12 +2453,6 @@
       <c r="B284" s="4" t="n">
         <v>43018</v>
       </c>
-      <c r="C284" s="0" t="n">
-        <v>65.4256419316842</v>
-      </c>
-      <c r="D284" s="0" t="n">
-        <v>65.3262645397</v>
-      </c>
     </row>
     <row r="285" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="3" t="n">
@@ -4159,12 +2461,6 @@
       <c r="B285" s="4" t="n">
         <v>43019</v>
       </c>
-      <c r="C285" s="0" t="n">
-        <v>65.4667634976525</v>
-      </c>
-      <c r="D285" s="0" t="n">
-        <v>65.3262645397</v>
-      </c>
     </row>
     <row r="286" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="3" t="n">
@@ -4173,12 +2469,6 @@
       <c r="B286" s="4" t="n">
         <v>43020</v>
       </c>
-      <c r="C286" s="0" t="n">
-        <v>65.478144736842</v>
-      </c>
-      <c r="D286" s="0" t="n">
-        <v>65.3262645397</v>
-      </c>
     </row>
     <row r="287" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="3" t="n">
@@ -4187,12 +2477,6 @@
       <c r="B287" s="4" t="n">
         <v>43021</v>
       </c>
-      <c r="C287" s="0" t="n">
-        <v>65.4859950466199</v>
-      </c>
-      <c r="D287" s="0" t="n">
-        <v>65.3262645397</v>
-      </c>
     </row>
     <row r="288" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="3" t="n">
@@ -4201,12 +2485,6 @@
       <c r="B288" s="4" t="n">
         <v>43022</v>
       </c>
-      <c r="C288" s="0" t="n">
-        <v>65.5060583623692</v>
-      </c>
-      <c r="D288" s="0" t="n">
-        <v>65.3262645397</v>
-      </c>
     </row>
     <row r="289" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="3" t="n">
@@ -4215,12 +2493,6 @@
       <c r="B289" s="4" t="n">
         <v>43023</v>
       </c>
-      <c r="C289" s="0" t="n">
-        <v>65.5210836226851</v>
-      </c>
-      <c r="D289" s="0" t="n">
-        <v>65.3262645397</v>
-      </c>
     </row>
     <row r="290" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="3" t="n">
@@ -4229,12 +2501,6 @@
       <c r="B290" s="4" t="n">
         <v>43024</v>
       </c>
-      <c r="C290" s="0" t="n">
-        <v>65.4991335063436</v>
-      </c>
-      <c r="D290" s="0" t="n">
-        <v>65.3262645397</v>
-      </c>
     </row>
     <row r="291" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="3" t="n">
@@ -4243,12 +2509,6 @@
       <c r="B291" s="4" t="n">
         <v>43025</v>
       </c>
-      <c r="C291" s="0" t="n">
-        <v>65.4637499999999</v>
-      </c>
-      <c r="D291" s="0" t="n">
-        <v>65.3262645397</v>
-      </c>
     </row>
     <row r="292" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="3" t="n">
@@ -4257,12 +2517,6 @@
       <c r="B292" s="4" t="n">
         <v>43026</v>
       </c>
-      <c r="C292" s="0" t="n">
-        <v>65.4304610538372</v>
-      </c>
-      <c r="D292" s="0" t="n">
-        <v>65.3262645397</v>
-      </c>
     </row>
     <row r="293" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A293" s="3" t="n">
@@ -4271,12 +2525,6 @@
       <c r="B293" s="4" t="n">
         <v>43027</v>
       </c>
-      <c r="C293" s="0" t="n">
-        <v>65.4037086187214</v>
-      </c>
-      <c r="D293" s="0" t="n">
-        <v>65.3262645397</v>
-      </c>
     </row>
     <row r="294" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A294" s="3" t="n">
@@ -4285,12 +2533,6 @@
       <c r="B294" s="4" t="n">
         <v>43028</v>
       </c>
-      <c r="C294" s="0" t="n">
-        <v>65.3791979522183</v>
-      </c>
-      <c r="D294" s="0" t="n">
-        <v>65.3262645397</v>
-      </c>
     </row>
     <row r="295" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A295" s="3" t="n">
@@ -4299,12 +2541,6 @@
       <c r="B295" s="4" t="n">
         <v>43029</v>
       </c>
-      <c r="C295" s="0" t="n">
-        <v>65.3675836167799</v>
-      </c>
-      <c r="D295" s="0" t="n">
-        <v>65.3262645397</v>
-      </c>
     </row>
     <row r="296" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A296" s="3" t="n">
@@ -4313,12 +2549,6 @@
       <c r="B296" s="4" t="n">
         <v>43030</v>
       </c>
-      <c r="C296" s="0" t="n">
-        <v>65.3672683615818</v>
-      </c>
-      <c r="D296" s="0" t="n">
-        <v>65.3262645397</v>
-      </c>
     </row>
     <row r="297" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A297" s="3" t="n">
@@ -4327,12 +2557,6 @@
       <c r="B297" s="4" t="n">
         <v>43031</v>
       </c>
-      <c r="C297" s="0" t="n">
-        <v>65.3682713963963</v>
-      </c>
-      <c r="D297" s="0" t="n">
-        <v>65.3262645397</v>
-      </c>
     </row>
     <row r="298" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="3" t="n">
@@ -4341,12 +2565,6 @@
       <c r="B298" s="4" t="n">
         <v>43032</v>
       </c>
-      <c r="C298" s="0" t="n">
-        <v>65.332079124579</v>
-      </c>
-      <c r="D298" s="0" t="n">
-        <v>65.3262645397</v>
-      </c>
     </row>
     <row r="299" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="3" t="n">
@@ -4355,12 +2573,6 @@
       <c r="B299" s="4" t="n">
         <v>43033</v>
       </c>
-      <c r="C299" s="0" t="n">
-        <v>65.2808808724831</v>
-      </c>
-      <c r="D299" s="0" t="n">
-        <v>65.3262645397</v>
-      </c>
     </row>
     <row r="300" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="3" t="n">
@@ -4369,12 +2581,6 @@
       <c r="B300" s="4" t="n">
         <v>43034</v>
       </c>
-      <c r="C300" s="0" t="n">
-        <v>65.2328720735785</v>
-      </c>
-      <c r="D300" s="0" t="n">
-        <v>65.3262645397</v>
-      </c>
     </row>
     <row r="301" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A301" s="3" t="n">
@@ -4383,12 +2589,6 @@
       <c r="B301" s="4" t="n">
         <v>43035</v>
       </c>
-      <c r="C301" s="0" t="n">
-        <v>65.2092902777777</v>
-      </c>
-      <c r="D301" s="0" t="n">
-        <v>65.3262645397</v>
-      </c>
     </row>
     <row r="302" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="3" t="n">
@@ -4397,12 +2597,6 @@
       <c r="B302" s="4" t="n">
         <v>43036</v>
       </c>
-      <c r="C302" s="0" t="n">
-        <v>65.1651328903653</v>
-      </c>
-      <c r="D302" s="0" t="n">
-        <v>65.3262645397</v>
-      </c>
     </row>
     <row r="303" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A303" s="3" t="n">
@@ -4411,12 +2605,6 @@
       <c r="B303" s="4" t="n">
         <v>43037</v>
       </c>
-      <c r="C303" s="0" t="n">
-        <v>65.0797778697571</v>
-      </c>
-      <c r="D303" s="0" t="n">
-        <v>65.3262645397</v>
-      </c>
     </row>
     <row r="304" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="3" t="n">
@@ -4425,12 +2613,6 @@
       <c r="B304" s="4" t="n">
         <v>43038</v>
       </c>
-      <c r="C304" s="0" t="n">
-        <v>65.0082728272826</v>
-      </c>
-      <c r="D304" s="0" t="n">
-        <v>65.3262645397</v>
-      </c>
     </row>
     <row r="305" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A305" s="3" t="n">
@@ -4439,12 +2621,6 @@
       <c r="B305" s="4" t="n">
         <v>43039</v>
       </c>
-      <c r="C305" s="0" t="n">
-        <v>64.9679851973683</v>
-      </c>
-      <c r="D305" s="0" t="n">
-        <v>65.3262645397</v>
-      </c>
     </row>
     <row r="306" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="3" t="n">
@@ -4453,12 +2629,6 @@
       <c r="B306" s="4" t="n">
         <v>43040</v>
       </c>
-      <c r="C306" s="0" t="n">
-        <v>64.9322868852458</v>
-      </c>
-      <c r="D306" s="0" t="n">
-        <v>64.50844855</v>
-      </c>
     </row>
     <row r="307" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A307" s="3" t="n">
@@ -4467,12 +2637,6 @@
       <c r="B307" s="4" t="n">
         <v>43041</v>
       </c>
-      <c r="C307" s="0" t="n">
-        <v>64.9227750544661</v>
-      </c>
-      <c r="D307" s="0" t="n">
-        <v>64.50844855</v>
-      </c>
     </row>
     <row r="308" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A308" s="3" t="n">
@@ -4481,12 +2645,6 @@
       <c r="B308" s="4" t="n">
         <v>43042</v>
       </c>
-      <c r="C308" s="0" t="n">
-        <v>64.9259310532029</v>
-      </c>
-      <c r="D308" s="0" t="n">
-        <v>64.50844855</v>
-      </c>
     </row>
     <row r="309" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A309" s="3" t="n">
@@ -4495,12 +2653,6 @@
       <c r="B309" s="4" t="n">
         <v>43043</v>
       </c>
-      <c r="C309" s="0" t="n">
-        <v>64.9318966450215</v>
-      </c>
-      <c r="D309" s="0" t="n">
-        <v>64.50844855</v>
-      </c>
     </row>
     <row r="310" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A310" s="3" t="n">
@@ -4509,12 +2661,6 @@
       <c r="B310" s="4" t="n">
         <v>43044</v>
       </c>
-      <c r="C310" s="0" t="n">
-        <v>64.9399271844659</v>
-      </c>
-      <c r="D310" s="0" t="n">
-        <v>64.50844855</v>
-      </c>
     </row>
     <row r="311" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A311" s="3" t="n">
@@ -4523,12 +2669,6 @@
       <c r="B311" s="4" t="n">
         <v>43045</v>
       </c>
-      <c r="C311" s="0" t="n">
-        <v>64.948067204301</v>
-      </c>
-      <c r="D311" s="0" t="n">
-        <v>64.50844855</v>
-      </c>
     </row>
     <row r="312" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="3" t="n">
@@ -4537,12 +2677,6 @@
       <c r="B312" s="4" t="n">
         <v>43046</v>
       </c>
-      <c r="C312" s="0" t="n">
-        <v>64.9543542336548</v>
-      </c>
-      <c r="D312" s="0" t="n">
-        <v>64.50844855</v>
-      </c>
     </row>
     <row r="313" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A313" s="3" t="n">
@@ -4551,12 +2685,6 @@
       <c r="B313" s="4" t="n">
         <v>43047</v>
       </c>
-      <c r="C313" s="0" t="n">
-        <v>64.917923344017</v>
-      </c>
-      <c r="D313" s="0" t="n">
-        <v>64.50844855</v>
-      </c>
     </row>
     <row r="314" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A314" s="3" t="n">
@@ -4565,12 +2693,6 @@
       <c r="B314" s="4" t="n">
         <v>43048</v>
       </c>
-      <c r="C314" s="0" t="n">
-        <v>64.8748628860489</v>
-      </c>
-      <c r="D314" s="0" t="n">
-        <v>64.50844855</v>
-      </c>
     </row>
     <row r="315" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A315" s="3" t="n">
@@ -4579,12 +2701,6 @@
       <c r="B315" s="4" t="n">
         <v>43049</v>
       </c>
-      <c r="C315" s="0" t="n">
-        <v>64.8214450636942</v>
-      </c>
-      <c r="D315" s="0" t="n">
-        <v>64.50844855</v>
-      </c>
     </row>
     <row r="316" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A316" s="3" t="n">
@@ -4593,12 +2709,6 @@
       <c r="B316" s="4" t="n">
         <v>43050</v>
       </c>
-      <c r="C316" s="0" t="n">
-        <v>64.7623835978835</v>
-      </c>
-      <c r="D316" s="0" t="n">
-        <v>64.50844855</v>
-      </c>
     </row>
     <row r="317" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A317" s="3" t="n">
@@ -4607,12 +2717,6 @@
       <c r="B317" s="4" t="n">
         <v>43051</v>
       </c>
-      <c r="C317" s="0" t="n">
-        <v>64.7204258966243</v>
-      </c>
-      <c r="D317" s="0" t="n">
-        <v>64.50844855</v>
-      </c>
     </row>
     <row r="318" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A318" s="3" t="n">
@@ -4621,12 +2725,6 @@
       <c r="B318" s="4" t="n">
         <v>43052</v>
       </c>
-      <c r="C318" s="0" t="n">
-        <v>64.6787920609883</v>
-      </c>
-      <c r="D318" s="0" t="n">
-        <v>64.50844855</v>
-      </c>
     </row>
     <row r="319" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A319" s="3" t="n">
@@ -4635,12 +2733,6 @@
       <c r="B319" s="4" t="n">
         <v>43053</v>
       </c>
-      <c r="C319" s="0" t="n">
-        <v>64.621823899371</v>
-      </c>
-      <c r="D319" s="0" t="n">
-        <v>64.50844855</v>
-      </c>
     </row>
     <row r="320" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A320" s="3" t="n">
@@ -4649,12 +2741,6 @@
       <c r="B320" s="4" t="n">
         <v>43054</v>
       </c>
-      <c r="C320" s="0" t="n">
-        <v>64.5696643155694</v>
-      </c>
-      <c r="D320" s="0" t="n">
-        <v>64.50844855</v>
-      </c>
     </row>
     <row r="321" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A321" s="3" t="n">
@@ -4663,12 +2749,6 @@
       <c r="B321" s="4" t="n">
         <v>43055</v>
       </c>
-      <c r="C321" s="0" t="n">
-        <v>64.5392643229166</v>
-      </c>
-      <c r="D321" s="0" t="n">
-        <v>64.50844855</v>
-      </c>
     </row>
     <row r="322" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A322" s="3" t="n">
@@ -4677,12 +2757,6 @@
       <c r="B322" s="4" t="n">
         <v>43056</v>
       </c>
-      <c r="C322" s="0" t="n">
-        <v>64.4928128245067</v>
-      </c>
-      <c r="D322" s="0" t="n">
-        <v>64.50844855</v>
-      </c>
     </row>
     <row r="323" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A323" s="3" t="n">
@@ -4691,12 +2765,6 @@
       <c r="B323" s="4" t="n">
         <v>43057</v>
       </c>
-      <c r="C323" s="0" t="n">
-        <v>64.4721752070392</v>
-      </c>
-      <c r="D323" s="0" t="n">
-        <v>64.50844855</v>
-      </c>
     </row>
     <row r="324" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A324" s="3" t="n">
@@ -4705,12 +2773,6 @@
       <c r="B324" s="4" t="n">
         <v>43058</v>
       </c>
-      <c r="C324" s="0" t="n">
-        <v>64.4126547987615</v>
-      </c>
-      <c r="D324" s="0" t="n">
-        <v>64.50844855</v>
-      </c>
     </row>
     <row r="325" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A325" s="3" t="n">
@@ -4719,12 +2781,6 @@
       <c r="B325" s="4" t="n">
         <v>43059</v>
       </c>
-      <c r="C325" s="0" t="n">
-        <v>64.3362101337447</v>
-      </c>
-      <c r="D325" s="0" t="n">
-        <v>64.50844855</v>
-      </c>
     </row>
     <row r="326" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A326" s="3" t="n">
@@ -4733,12 +2789,6 @@
       <c r="B326" s="4" t="n">
         <v>43060</v>
       </c>
-      <c r="C326" s="0" t="n">
-        <v>64.2840371794871</v>
-      </c>
-      <c r="D326" s="0" t="n">
-        <v>64.50844855</v>
-      </c>
     </row>
     <row r="327" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A327" s="3" t="n">
@@ -4747,12 +2797,6 @@
       <c r="B327" s="4" t="n">
         <v>43061</v>
       </c>
-      <c r="C327" s="0" t="n">
-        <v>64.2342446319017</v>
-      </c>
-      <c r="D327" s="0" t="n">
-        <v>64.50844855</v>
-      </c>
     </row>
     <row r="328" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A328" s="3" t="n">
@@ -4761,12 +2805,6 @@
       <c r="B328" s="4" t="n">
         <v>43062</v>
       </c>
-      <c r="C328" s="0" t="n">
-        <v>64.1665736493373</v>
-      </c>
-      <c r="D328" s="0" t="n">
-        <v>64.50844855</v>
-      </c>
     </row>
     <row r="329" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A329" s="3" t="n">
@@ -4775,12 +2813,6 @@
       <c r="B329" s="4" t="n">
         <v>43063</v>
       </c>
-      <c r="C329" s="0" t="n">
-        <v>64.1087677845527</v>
-      </c>
-      <c r="D329" s="0" t="n">
-        <v>64.50844855</v>
-      </c>
     </row>
     <row r="330" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A330" s="3" t="n">
@@ -4789,12 +2821,6 @@
       <c r="B330" s="4" t="n">
         <v>43064</v>
       </c>
-      <c r="C330" s="0" t="n">
-        <v>64.0679787234041</v>
-      </c>
-      <c r="D330" s="0" t="n">
-        <v>64.50844855</v>
-      </c>
     </row>
     <row r="331" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A331" s="3" t="n">
@@ -4803,12 +2829,6 @@
       <c r="B331" s="4" t="n">
         <v>43065</v>
       </c>
-      <c r="C331" s="0" t="n">
-        <v>64.025957070707</v>
-      </c>
-      <c r="D331" s="0" t="n">
-        <v>64.50844855</v>
-      </c>
     </row>
     <row r="332" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A332" s="3" t="n">
@@ -4817,12 +2837,6 @@
       <c r="B332" s="4" t="n">
         <v>43066</v>
       </c>
-      <c r="C332" s="0" t="n">
-        <v>63.9661555891238</v>
-      </c>
-      <c r="D332" s="0" t="n">
-        <v>64.50844855</v>
-      </c>
     </row>
     <row r="333" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A333" s="3" t="n">
@@ -4831,12 +2845,6 @@
       <c r="B333" s="4" t="n">
         <v>43067</v>
       </c>
-      <c r="C333" s="0" t="n">
-        <v>63.9130496987951</v>
-      </c>
-      <c r="D333" s="0" t="n">
-        <v>64.50844855</v>
-      </c>
     </row>
     <row r="334" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A334" s="3" t="n">
@@ -4845,12 +2853,6 @@
       <c r="B334" s="4" t="n">
         <v>43068</v>
       </c>
-      <c r="C334" s="0" t="n">
-        <v>63.8709234234233</v>
-      </c>
-      <c r="D334" s="0" t="n">
-        <v>64.50844855</v>
-      </c>
     </row>
     <row r="335" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A335" s="3" t="n">
@@ -4859,12 +2861,6 @@
       <c r="B335" s="4" t="n">
         <v>43069</v>
       </c>
-      <c r="C335" s="0" t="n">
-        <v>63.8399812874251</v>
-      </c>
-      <c r="D335" s="0" t="n">
-        <v>64.50844855</v>
-      </c>
     </row>
     <row r="336" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A336" s="3" t="n">
@@ -4873,12 +2869,6 @@
       <c r="B336" s="4" t="n">
         <v>43070</v>
       </c>
-      <c r="C336" s="0" t="n">
-        <v>63.8178893034825</v>
-      </c>
-      <c r="D336" s="0" t="n">
-        <v>62.962871592</v>
-      </c>
     </row>
     <row r="337" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A337" s="3" t="n">
@@ -4887,12 +2877,6 @@
       <c r="B337" s="4" t="n">
         <v>43071</v>
       </c>
-      <c r="C337" s="0" t="n">
-        <v>63.7840277777777</v>
-      </c>
-      <c r="D337" s="0" t="n">
-        <v>62.962871592</v>
-      </c>
     </row>
     <row r="338" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A338" s="3" t="n">
@@ -4901,12 +2885,6 @@
       <c r="B338" s="4" t="n">
         <v>43072</v>
       </c>
-      <c r="C338" s="0" t="n">
-        <v>63.7472576656775</v>
-      </c>
-      <c r="D338" s="0" t="n">
-        <v>62.962871592</v>
-      </c>
     </row>
     <row r="339" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A339" s="3" t="n">
@@ -4915,12 +2893,6 @@
       <c r="B339" s="4" t="n">
         <v>43073</v>
       </c>
-      <c r="C339" s="0" t="n">
-        <v>63.7130522682445</v>
-      </c>
-      <c r="D339" s="0" t="n">
-        <v>62.962871592</v>
-      </c>
     </row>
     <row r="340" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A340" s="3" t="n">
@@ -4929,12 +2901,6 @@
       <c r="B340" s="4" t="n">
         <v>43074</v>
       </c>
-      <c r="C340" s="0" t="n">
-        <v>63.6917551622418</v>
-      </c>
-      <c r="D340" s="0" t="n">
-        <v>62.962871592</v>
-      </c>
     </row>
     <row r="341" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A341" s="3" t="n">
@@ -4943,12 +2909,6 @@
       <c r="B341" s="4" t="n">
         <v>43075</v>
       </c>
-      <c r="C341" s="0" t="n">
-        <v>63.6233124999999</v>
-      </c>
-      <c r="D341" s="0" t="n">
-        <v>62.962871592</v>
-      </c>
     </row>
     <row r="342" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A342" s="3" t="n">
@@ -4957,12 +2917,6 @@
       <c r="B342" s="4" t="n">
         <v>43076</v>
       </c>
-      <c r="C342" s="0" t="n">
-        <v>63.559544232649</v>
-      </c>
-      <c r="D342" s="0" t="n">
-        <v>62.962871592</v>
-      </c>
     </row>
     <row r="343" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A343" s="3" t="n">
@@ -4971,12 +2925,6 @@
       <c r="B343" s="4" t="n">
         <v>43077</v>
       </c>
-      <c r="C343" s="0" t="n">
-        <v>63.4732370857699</v>
-      </c>
-      <c r="D343" s="0" t="n">
-        <v>62.962871592</v>
-      </c>
     </row>
     <row r="344" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A344" s="3" t="n">
@@ -4985,12 +2933,6 @@
       <c r="B344" s="4" t="n">
         <v>43078</v>
       </c>
-      <c r="C344" s="0" t="n">
-        <v>63.3914674441204</v>
-      </c>
-      <c r="D344" s="0" t="n">
-        <v>62.962871592</v>
-      </c>
     </row>
     <row r="345" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A345" s="3" t="n">
@@ -4999,12 +2941,6 @@
       <c r="B345" s="4" t="n">
         <v>43079</v>
       </c>
-      <c r="C345" s="0" t="n">
-        <v>63.3080486918604</v>
-      </c>
-      <c r="D345" s="0" t="n">
-        <v>62.962871592</v>
-      </c>
     </row>
     <row r="346" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A346" s="3" t="n">
@@ -5013,12 +2949,6 @@
       <c r="B346" s="4" t="n">
         <v>43080</v>
       </c>
-      <c r="C346" s="0" t="n">
-        <v>63.2445169082125</v>
-      </c>
-      <c r="D346" s="0" t="n">
-        <v>62.962871592</v>
-      </c>
     </row>
     <row r="347" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A347" s="3" t="n">
@@ -5027,12 +2957,6 @@
       <c r="B347" s="4" t="n">
         <v>43081</v>
       </c>
-      <c r="C347" s="0" t="n">
-        <v>63.1839788053949</v>
-      </c>
-      <c r="D347" s="0" t="n">
-        <v>62.962871592</v>
-      </c>
     </row>
     <row r="348" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A348" s="3" t="n">
@@ -5041,12 +2965,6 @@
       <c r="B348" s="4" t="n">
         <v>43082</v>
       </c>
-      <c r="C348" s="0" t="n">
-        <v>63.1009690201728</v>
-      </c>
-      <c r="D348" s="0" t="n">
-        <v>62.962871592</v>
-      </c>
     </row>
     <row r="349" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A349" s="3" t="n">
@@ -5055,12 +2973,6 @@
       <c r="B349" s="4" t="n">
         <v>43083</v>
       </c>
-      <c r="C349" s="0" t="n">
-        <v>63.041265565134</v>
-      </c>
-      <c r="D349" s="0" t="n">
-        <v>62.962871592</v>
-      </c>
     </row>
     <row r="350" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A350" s="3" t="n">
@@ -5069,12 +2981,6 @@
       <c r="B350" s="4" t="n">
         <v>43084</v>
       </c>
-      <c r="C350" s="0" t="n">
-        <v>62.9537655205348</v>
-      </c>
-      <c r="D350" s="0" t="n">
-        <v>62.962871592</v>
-      </c>
     </row>
     <row r="351" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A351" s="3" t="n">
@@ -5083,12 +2989,6 @@
       <c r="B351" s="4" t="n">
         <v>43085</v>
       </c>
-      <c r="C351" s="0" t="n">
-        <v>62.8717761904761</v>
-      </c>
-      <c r="D351" s="0" t="n">
-        <v>62.962871592</v>
-      </c>
     </row>
     <row r="352" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A352" s="3" t="n">
@@ -5097,12 +2997,6 @@
       <c r="B352" s="4" t="n">
         <v>43086</v>
       </c>
-      <c r="C352" s="0" t="n">
-        <v>62.8002896486229</v>
-      </c>
-      <c r="D352" s="0" t="n">
-        <v>62.962871592</v>
-      </c>
     </row>
     <row r="353" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A353" s="3" t="n">
@@ -5111,12 +3005,6 @@
       <c r="B353" s="4" t="n">
         <v>43087</v>
       </c>
-      <c r="C353" s="0" t="n">
-        <v>62.7564902935605</v>
-      </c>
-      <c r="D353" s="0" t="n">
-        <v>62.962871592</v>
-      </c>
     </row>
     <row r="354" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A354" s="3" t="n">
@@ -5125,12 +3013,6 @@
       <c r="B354" s="4" t="n">
         <v>43088</v>
       </c>
-      <c r="C354" s="0" t="n">
-        <v>62.7194865439092</v>
-      </c>
-      <c r="D354" s="0" t="n">
-        <v>62.962871592</v>
-      </c>
     </row>
     <row r="355" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A355" s="3" t="n">
@@ -5139,12 +3021,6 @@
       <c r="B355" s="4" t="n">
         <v>43089</v>
       </c>
-      <c r="C355" s="0" t="n">
-        <v>62.7004119585686</v>
-      </c>
-      <c r="D355" s="0" t="n">
-        <v>62.962871592</v>
-      </c>
     </row>
     <row r="356" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A356" s="3" t="n">
@@ -5153,12 +3029,6 @@
       <c r="B356" s="4" t="n">
         <v>43090</v>
       </c>
-      <c r="C356" s="0" t="n">
-        <v>62.6750622065727</v>
-      </c>
-      <c r="D356" s="0" t="n">
-        <v>62.962871592</v>
-      </c>
     </row>
     <row r="357" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A357" s="3" t="n">
@@ -5167,12 +3037,6 @@
       <c r="B357" s="4" t="n">
         <v>43091</v>
       </c>
-      <c r="C357" s="0" t="n">
-        <v>62.6511060393257</v>
-      </c>
-      <c r="D357" s="0" t="n">
-        <v>62.962871592</v>
-      </c>
     </row>
     <row r="358" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A358" s="3" t="n">
@@ -5181,12 +3045,6 @@
       <c r="B358" s="4" t="n">
         <v>43092</v>
       </c>
-      <c r="C358" s="0" t="n">
-        <v>62.6371486928103</v>
-      </c>
-      <c r="D358" s="0" t="n">
-        <v>62.962871592</v>
-      </c>
     </row>
     <row r="359" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A359" s="3" t="n">
@@ -5195,12 +3053,6 @@
       <c r="B359" s="4" t="n">
         <v>43093</v>
       </c>
-      <c r="C359" s="0" t="n">
-        <v>62.5869785847298</v>
-      </c>
-      <c r="D359" s="0" t="n">
-        <v>62.962871592</v>
-      </c>
     </row>
     <row r="360" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A360" s="3" t="n">
@@ -5209,12 +3061,6 @@
       <c r="B360" s="4" t="n">
         <v>43094</v>
       </c>
-      <c r="C360" s="0" t="n">
-        <v>62.5000441039924</v>
-      </c>
-      <c r="D360" s="0" t="n">
-        <v>62.962871592</v>
-      </c>
     </row>
     <row r="361" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A361" s="3" t="n">
@@ -5223,12 +3069,6 @@
       <c r="B361" s="4" t="n">
         <v>43095</v>
       </c>
-      <c r="C361" s="0" t="n">
-        <v>62.4229594907406</v>
-      </c>
-      <c r="D361" s="0" t="n">
-        <v>62.962871592</v>
-      </c>
     </row>
     <row r="362" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A362" s="3" t="n">
@@ -5237,12 +3077,6 @@
       <c r="B362" s="4" t="n">
         <v>43096</v>
       </c>
-      <c r="C362" s="0" t="n">
-        <v>62.3410087719297</v>
-      </c>
-      <c r="D362" s="0" t="n">
-        <v>62.962871592</v>
-      </c>
     </row>
     <row r="363" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A363" s="3" t="n">
@@ -5251,12 +3085,6 @@
       <c r="B363" s="4" t="n">
         <v>43097</v>
       </c>
-      <c r="C363" s="0" t="n">
-        <v>62.250888581952</v>
-      </c>
-      <c r="D363" s="0" t="n">
-        <v>62.962871592</v>
-      </c>
     </row>
     <row r="364" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A364" s="3" t="n">
@@ -5265,12 +3093,6 @@
       <c r="B364" s="4" t="n">
         <v>43098</v>
       </c>
-      <c r="C364" s="0" t="n">
-        <v>62.1798748852157</v>
-      </c>
-      <c r="D364" s="0" t="n">
-        <v>62.962871592</v>
-      </c>
     </row>
     <row r="365" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A365" s="3" t="n">
@@ -5279,12 +3101,6 @@
       <c r="B365" s="4" t="n">
         <v>43099</v>
       </c>
-      <c r="C365" s="0" t="n">
-        <v>62.1063576007325</v>
-      </c>
-      <c r="D365" s="0" t="n">
-        <v>62.962871592</v>
-      </c>
     </row>
     <row r="366" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A366" s="3" t="n">
@@ -5293,17 +3109,11 @@
       <c r="B366" s="4" t="n">
         <v>43100</v>
       </c>
-      <c r="C366" s="0" t="n">
-        <v>62.0156678082191</v>
-      </c>
-      <c r="D366" s="0" t="n">
-        <v>62.962871592</v>
-      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>